<commit_message>
Zero out transit simple delay
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDB076-3820-4052-953E-0A38B15132FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
     <sheet name="transitLineToVehicle" sheetId="1" r:id="rId2"/>
     <sheet name="transitVehicleToCapacity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3215,7 +3224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4084,7 +4093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4822,12 +4831,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17927,12 +17936,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18248,7 +18257,7 @@
         <v>173</v>
       </c>
       <c r="E12" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0.122</v>
@@ -18274,7 +18283,7 @@
         <v>1047</v>
       </c>
       <c r="E13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <v>0.122</v>
@@ -18300,7 +18309,7 @@
         <v>91</v>
       </c>
       <c r="E14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18326,7 +18335,7 @@
         <v>287</v>
       </c>
       <c r="E15" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -18404,7 +18413,7 @@
         <v>328</v>
       </c>
       <c r="E18" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -18430,7 +18439,7 @@
         <v>333</v>
       </c>
       <c r="E19" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -18456,7 +18465,7 @@
         <v>1046</v>
       </c>
       <c r="E20" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -18482,7 +18491,7 @@
         <v>1045</v>
       </c>
       <c r="E21" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -18508,7 +18517,7 @@
         <v>1044</v>
       </c>
       <c r="E22" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -18534,7 +18543,7 @@
         <v>265</v>
       </c>
       <c r="E23" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>0.122</v>
@@ -18560,7 +18569,7 @@
         <v>217</v>
       </c>
       <c r="E24" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
         <v>0.122</v>
@@ -18586,7 +18595,7 @@
         <v>1043</v>
       </c>
       <c r="E25" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1">
         <v>0.122</v>
@@ -18612,7 +18621,7 @@
         <v>224</v>
       </c>
       <c r="E26" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1">
         <v>0.10199999999999999</v>
@@ -18638,7 +18647,7 @@
         <v>1042</v>
       </c>
       <c r="E27" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
         <v>0.10199999999999999</v>
@@ -18664,7 +18673,7 @@
         <v>1041</v>
       </c>
       <c r="E28" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
         <v>0.10199999999999999</v>
@@ -18690,7 +18699,7 @@
         <v>261</v>
       </c>
       <c r="E29" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F29" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18716,7 +18725,7 @@
         <v>230</v>
       </c>
       <c r="E30" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F30" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18742,7 +18751,7 @@
         <v>1040</v>
       </c>
       <c r="E31" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18768,7 +18777,7 @@
         <v>205</v>
       </c>
       <c r="E32" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18794,7 +18803,7 @@
         <v>207</v>
       </c>
       <c r="E33" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18820,7 +18829,7 @@
         <v>1039</v>
       </c>
       <c r="E34" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18846,7 +18855,7 @@
         <v>36</v>
       </c>
       <c r="E35" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
         <v>0.122</v>
@@ -18872,7 +18881,7 @@
         <v>53</v>
       </c>
       <c r="E36" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
         <v>8.2000000000000003E-2</v>
@@ -18898,7 +18907,7 @@
         <v>325</v>
       </c>
       <c r="E37" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -18924,7 +18933,7 @@
         <v>245</v>
       </c>
       <c r="E38" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
         <v>0.122</v>
@@ -18950,7 +18959,7 @@
         <v>215</v>
       </c>
       <c r="E39" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1">
         <v>0.122</v>
@@ -18976,7 +18985,7 @@
         <v>1038</v>
       </c>
       <c r="E40" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
         <v>0.122</v>
@@ -19002,7 +19011,7 @@
         <v>234</v>
       </c>
       <c r="E41" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F41" s="1">
         <v>8.2000000000000003E-2</v>
@@ -19028,7 +19037,7 @@
         <v>235</v>
       </c>
       <c r="E42" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
         <v>8.2000000000000003E-2</v>
@@ -19054,7 +19063,7 @@
         <v>1037</v>
       </c>
       <c r="E43" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1">
         <v>8.2000000000000003E-2</v>
@@ -19106,7 +19115,7 @@
         <v>259</v>
       </c>
       <c r="E45" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -19132,7 +19141,7 @@
         <v>1036</v>
       </c>
       <c r="E46" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Add HSR capacity info to TransitCapacity.xlsx
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBDB076-3820-4052-953E-0A38B15132FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
     <sheet name="transitLineToVehicle" sheetId="1" r:id="rId2"/>
     <sheet name="transitVehicleToCapacity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3555" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1079">
   <si>
     <t>Name</t>
   </si>
@@ -3219,12 +3218,60 @@
   </si>
   <si>
     <t>120_RED-</t>
+  </si>
+  <si>
+    <t>137_A</t>
+  </si>
+  <si>
+    <t>137_B</t>
+  </si>
+  <si>
+    <t>137_C</t>
+  </si>
+  <si>
+    <t>HSR</t>
+  </si>
+  <si>
+    <t>SFG</t>
+  </si>
+  <si>
+    <t>SFSJ</t>
+  </si>
+  <si>
+    <t>SJG</t>
+  </si>
+  <si>
+    <t>SF - GILROY</t>
+  </si>
+  <si>
+    <t>SF - SAN JOSE</t>
+  </si>
+  <si>
+    <t>SAM JOSE - GILROY</t>
+  </si>
+  <si>
+    <t>HSR6</t>
+  </si>
+  <si>
+    <t>HSR4</t>
+  </si>
+  <si>
+    <t>HSR10</t>
+  </si>
+  <si>
+    <t>HSR 4 trains</t>
+  </si>
+  <si>
+    <t>HSR 6 trains</t>
+  </si>
+  <si>
+    <t>HSR 10 trains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4093,12 +4140,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4821,7 +4868,7 @@
         <v>909</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>908</v>
+        <v>1066</v>
       </c>
     </row>
   </sheetData>
@@ -4831,12 +4878,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H492"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <pane ySplit="1" topLeftCell="A456" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17425,7 +17472,7 @@
         <v>203</v>
       </c>
       <c r="C474" s="4" t="str">
-        <f t="shared" ref="C474:C491" si="14">RIGHT($A474,LEN($A474)-FIND("_",$A474))</f>
+        <f t="shared" ref="C474:C494" si="14">RIGHT($A474,LEN($A474)-FIND("_",$A474))</f>
         <v>L</v>
       </c>
       <c r="D474" s="12" t="s">
@@ -17904,28 +17951,109 @@
       </c>
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A492" s="1" t="s">
+      <c r="A492" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B492" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C492" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v>A</v>
+      </c>
+      <c r="D492" s="11" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E492" s="6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F492" s="6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G492" s="6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H492" s="6" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A493" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B493" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C493" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>B</v>
+      </c>
+      <c r="D493" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E493" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F493" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G493" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H493" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A494" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B494" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C494" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>C</v>
+      </c>
+      <c r="D494" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F494" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G494" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H494" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A495" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B492" s="1" t="s">
+      <c r="B495" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C492" s="1" t="s">
+      <c r="C495" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D492" s="9" t="s">
+      <c r="D495" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E492" s="1" t="s">
+      <c r="E495" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F492" s="1" t="s">
+      <c r="F495" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G492" s="1" t="s">
+      <c r="G495" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H492" s="1" t="s">
+      <c r="H495" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -17936,12 +18064,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19179,6 +19307,84 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1800</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1530</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2700</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2295</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3825</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Export transit capacity updates from workbook to csvs
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C736C-3FF0-407B-B6B4-A8A20F7C404A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
     <sheet name="transitLineToVehicle" sheetId="1" r:id="rId2"/>
     <sheet name="transitVehicleToCapacity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3271,7 +3272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4140,12 +4141,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4878,12 +4879,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A456" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H497" sqref="H497"/>
+      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A488" sqref="A488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18064,12 +18065,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update 28R line names in transitcapacity.xlsx
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C736C-3FF0-407B-B6B4-A8A20F7C404A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
     <sheet name="transitLineToVehicle" sheetId="1" r:id="rId2"/>
     <sheet name="transitVehicleToCapacity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511" iterateCount="10000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2153,12 +2152,6 @@
     <t>28 - 19th AVE</t>
   </si>
   <si>
-    <t>21_28RNB</t>
-  </si>
-  <si>
-    <t>21_28RSB</t>
-  </si>
-  <si>
     <t>28R - 19TH AVENUE RAPID</t>
   </si>
   <si>
@@ -3267,12 +3260,18 @@
   </si>
   <si>
     <t>HSR 10 trains</t>
+  </si>
+  <si>
+    <t>21_28RN</t>
+  </si>
+  <si>
+    <t>21_28RS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4141,10 +4140,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
@@ -4159,21 +4158,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>205</v>
@@ -4181,10 +4180,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>205</v>
@@ -4192,10 +4191,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>261</v>
@@ -4203,10 +4202,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>261</v>
@@ -4214,10 +4213,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>261</v>
@@ -4225,10 +4224,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>261</v>
@@ -4236,10 +4235,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>261</v>
@@ -4247,10 +4246,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>261</v>
@@ -4258,10 +4257,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>261</v>
@@ -4269,10 +4268,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>261</v>
@@ -4280,10 +4279,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>287</v>
@@ -4291,10 +4290,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>205</v>
@@ -4302,10 +4301,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>205</v>
@@ -4313,10 +4312,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>205</v>
@@ -4324,10 +4323,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>205</v>
@@ -4335,10 +4334,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>91</v>
@@ -4346,10 +4345,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>205</v>
@@ -4357,10 +4356,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>205</v>
@@ -4368,10 +4367,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>205</v>
@@ -4379,10 +4378,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>205</v>
@@ -4390,10 +4389,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>205</v>
@@ -4401,10 +4400,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>205</v>
@@ -4412,10 +4411,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>205</v>
@@ -4423,10 +4422,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>205</v>
@@ -4434,10 +4433,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>205</v>
@@ -4445,10 +4444,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>205</v>
@@ -4456,10 +4455,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>205</v>
@@ -4467,10 +4466,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>205</v>
@@ -4478,10 +4477,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>205</v>
@@ -4489,10 +4488,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>205</v>
@@ -4500,10 +4499,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>205</v>
@@ -4511,10 +4510,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>205</v>
@@ -4522,10 +4521,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>205</v>
@@ -4533,10 +4532,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>205</v>
@@ -4544,10 +4543,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>205</v>
@@ -4555,10 +4554,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>205</v>
@@ -4566,10 +4565,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>205</v>
@@ -4577,10 +4576,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>205</v>
@@ -4588,10 +4587,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>205</v>
@@ -4599,10 +4598,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>205</v>
@@ -4610,10 +4609,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>205</v>
@@ -4621,10 +4620,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>205</v>
@@ -4632,10 +4631,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>205</v>
@@ -4643,10 +4642,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>205</v>
@@ -4654,10 +4653,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>205</v>
@@ -4665,10 +4664,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>205</v>
@@ -4676,76 +4675,76 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>333</v>
@@ -4753,10 +4752,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>333</v>
@@ -4764,7 +4763,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>22</v>
@@ -4775,10 +4774,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>333</v>
@@ -4786,90 +4785,90 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
   </sheetData>
@@ -4879,12 +4878,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H495"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A488" sqref="A488"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5010,7 +5009,7 @@
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
@@ -5066,7 +5065,7 @@
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
@@ -5122,7 +5121,7 @@
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
@@ -5150,7 +5149,7 @@
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
@@ -5178,7 +5177,7 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
@@ -10555,7 +10554,7 @@
     </row>
     <row r="218" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>203</v>
@@ -10717,7 +10716,7 @@
     </row>
     <row r="224" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>203</v>
@@ -11095,20 +11094,20 @@
     </row>
     <row r="238" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>707</v>
+        <v>1077</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>203</v>
       </c>
       <c r="C238" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>28RNB</v>
+        <v>28RN</v>
       </c>
       <c r="D238" s="16" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F238" s="3" t="s">
         <v>205</v>
@@ -11122,20 +11121,20 @@
     </row>
     <row r="239" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>708</v>
+        <v>1078</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>203</v>
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>28RSB</v>
+        <v>28RS</v>
       </c>
       <c r="D239" s="16" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F239" s="3" t="s">
         <v>205</v>
@@ -11149,7 +11148,7 @@
     </row>
     <row r="240" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>203</v>
@@ -11230,7 +11229,7 @@
     </row>
     <row r="243" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>203</v>
@@ -11257,7 +11256,7 @@
     </row>
     <row r="244" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>203</v>
@@ -11284,7 +11283,7 @@
     </row>
     <row r="245" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>203</v>
@@ -11311,7 +11310,7 @@
     </row>
     <row r="246" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>203</v>
@@ -11338,7 +11337,7 @@
     </row>
     <row r="247" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>203</v>
@@ -11365,7 +11364,7 @@
     </row>
     <row r="248" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>203</v>
@@ -11392,7 +11391,7 @@
     </row>
     <row r="249" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>203</v>
@@ -11419,7 +11418,7 @@
     </row>
     <row r="250" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>203</v>
@@ -11446,7 +11445,7 @@
     </row>
     <row r="251" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>203</v>
@@ -11473,7 +11472,7 @@
     </row>
     <row r="252" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>203</v>
@@ -11500,7 +11499,7 @@
     </row>
     <row r="253" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>203</v>
@@ -11527,7 +11526,7 @@
     </row>
     <row r="254" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>203</v>
@@ -11554,7 +11553,7 @@
     </row>
     <row r="255" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>203</v>
@@ -11581,7 +11580,7 @@
     </row>
     <row r="256" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>203</v>
@@ -11591,10 +11590,10 @@
         <v>30XIN</v>
       </c>
       <c r="D256" s="16" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E256" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F256" s="3" t="s">
         <v>207</v>
@@ -11608,7 +11607,7 @@
     </row>
     <row r="257" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>203</v>
@@ -11618,10 +11617,10 @@
         <v>30XOUT</v>
       </c>
       <c r="D257" s="16" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F257" s="3" t="s">
         <v>207</v>
@@ -11635,7 +11634,7 @@
     </row>
     <row r="258" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>203</v>
@@ -11645,10 +11644,10 @@
         <v>31AXIN</v>
       </c>
       <c r="D258" s="16" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E258" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F258" s="3" t="s">
         <v>207</v>
@@ -11662,7 +11661,7 @@
     </row>
     <row r="259" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>203</v>
@@ -11672,10 +11671,10 @@
         <v>31AXOUT</v>
       </c>
       <c r="D259" s="16" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E259" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F259" s="3" t="s">
         <v>207</v>
@@ -11689,7 +11688,7 @@
     </row>
     <row r="260" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>203</v>
@@ -11699,10 +11698,10 @@
         <v>31BXIN</v>
       </c>
       <c r="D260" s="16" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E260" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F260" s="3" t="s">
         <v>207</v>
@@ -11716,7 +11715,7 @@
     </row>
     <row r="261" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>203</v>
@@ -11726,10 +11725,10 @@
         <v>31BXOUT</v>
       </c>
       <c r="D261" s="16" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F261" s="3" t="s">
         <v>207</v>
@@ -11743,7 +11742,7 @@
     </row>
     <row r="262" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>203</v>
@@ -11756,7 +11755,7 @@
         <v>31</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F262" s="3" t="s">
         <v>235</v>
@@ -11770,7 +11769,7 @@
     </row>
     <row r="263" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>203</v>
@@ -11783,7 +11782,7 @@
         <v>31</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F263" s="3" t="s">
         <v>235</v>
@@ -11797,7 +11796,7 @@
     </row>
     <row r="264" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>203</v>
@@ -11810,7 +11809,7 @@
         <v>31</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F264" s="3" t="s">
         <v>235</v>
@@ -11824,7 +11823,7 @@
     </row>
     <row r="265" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>203</v>
@@ -11837,7 +11836,7 @@
         <v>31</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F265" s="3" t="s">
         <v>235</v>
@@ -11905,7 +11904,7 @@
     </row>
     <row r="268" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>203</v>
@@ -11918,7 +11917,7 @@
         <v>33</v>
       </c>
       <c r="E268" s="3" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F268" s="3" t="s">
         <v>235</v>
@@ -11945,7 +11944,7 @@
         <v>33</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>235</v>
@@ -11972,7 +11971,7 @@
         <v>33</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>235</v>
@@ -12067,7 +12066,7 @@
     </row>
     <row r="274" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>203</v>
@@ -12080,7 +12079,7 @@
         <v>36</v>
       </c>
       <c r="E274" s="3" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F274" s="3" t="s">
         <v>230</v>
@@ -12107,7 +12106,7 @@
         <v>262</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>230</v>
@@ -12134,7 +12133,7 @@
         <v>263</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>230</v>
@@ -12148,7 +12147,7 @@
     </row>
     <row r="277" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B277" s="3" t="s">
         <v>203</v>
@@ -12161,7 +12160,7 @@
         <v>37</v>
       </c>
       <c r="E277" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F277" s="3" t="s">
         <v>230</v>
@@ -12188,7 +12187,7 @@
         <v>37</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>230</v>
@@ -12215,7 +12214,7 @@
         <v>37</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>230</v>
@@ -12229,7 +12228,7 @@
     </row>
     <row r="280" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>203</v>
@@ -12239,10 +12238,10 @@
         <v>38AXIN</v>
       </c>
       <c r="D280" s="16" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E280" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F280" s="3" t="s">
         <v>207</v>
@@ -12256,7 +12255,7 @@
     </row>
     <row r="281" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>203</v>
@@ -12266,10 +12265,10 @@
         <v>38AXOUT</v>
       </c>
       <c r="D281" s="16" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E281" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F281" s="3" t="s">
         <v>207</v>
@@ -12283,7 +12282,7 @@
     </row>
     <row r="282" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>203</v>
@@ -12293,10 +12292,10 @@
         <v>38BXIN</v>
       </c>
       <c r="D282" s="16" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E282" s="3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F282" s="3" t="s">
         <v>207</v>
@@ -12310,7 +12309,7 @@
     </row>
     <row r="283" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>203</v>
@@ -12320,10 +12319,10 @@
         <v>38BXOUT</v>
       </c>
       <c r="D283" s="16" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E283" s="3" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F283" s="3" t="s">
         <v>207</v>
@@ -12391,7 +12390,7 @@
     </row>
     <row r="286" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>203</v>
@@ -12418,7 +12417,7 @@
     </row>
     <row r="287" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>203</v>
@@ -12445,7 +12444,7 @@
     </row>
     <row r="288" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>203</v>
@@ -12472,7 +12471,7 @@
     </row>
     <row r="289" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>203</v>
@@ -12499,7 +12498,7 @@
     </row>
     <row r="290" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>203</v>
@@ -12512,7 +12511,7 @@
         <v>38</v>
       </c>
       <c r="E290" s="3" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F290" s="3" t="s">
         <v>265</v>
@@ -12526,7 +12525,7 @@
     </row>
     <row r="291" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>203</v>
@@ -12539,7 +12538,7 @@
         <v>38</v>
       </c>
       <c r="E291" s="3" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F291" s="3" t="s">
         <v>265</v>
@@ -12823,7 +12822,7 @@
     </row>
     <row r="302" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>203</v>
@@ -12836,7 +12835,7 @@
         <v>39</v>
       </c>
       <c r="E302" s="3" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F302" s="3" t="s">
         <v>230</v>
@@ -12850,7 +12849,7 @@
     </row>
     <row r="303" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B303" s="3" t="s">
         <v>203</v>
@@ -12863,7 +12862,7 @@
         <v>39</v>
       </c>
       <c r="E303" s="3" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F303" s="3" t="s">
         <v>230</v>
@@ -12877,7 +12876,7 @@
     </row>
     <row r="304" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B304" s="3" t="s">
         <v>203</v>
@@ -12890,7 +12889,7 @@
         <v>3</v>
       </c>
       <c r="E304" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="F304" s="3" t="s">
         <v>235</v>
@@ -12904,7 +12903,7 @@
     </row>
     <row r="305" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>203</v>
@@ -12917,7 +12916,7 @@
         <v>3</v>
       </c>
       <c r="E305" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="F305" s="3" t="s">
         <v>235</v>
@@ -12931,7 +12930,7 @@
     </row>
     <row r="306" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>203</v>
@@ -12944,7 +12943,7 @@
         <v>41</v>
       </c>
       <c r="E306" s="3" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F306" s="3" t="s">
         <v>235</v>
@@ -12958,7 +12957,7 @@
     </row>
     <row r="307" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>203</v>
@@ -12971,7 +12970,7 @@
         <v>41</v>
       </c>
       <c r="E307" s="3" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F307" s="3" t="s">
         <v>235</v>
@@ -13039,7 +13038,7 @@
     </row>
     <row r="310" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B310" s="3" t="s">
         <v>203</v>
@@ -13052,7 +13051,7 @@
         <v>43</v>
       </c>
       <c r="E310" s="3" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F310" s="3" t="s">
         <v>207</v>
@@ -13079,7 +13078,7 @@
         <v>43</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F311" s="1" t="s">
         <v>207</v>
@@ -13106,7 +13105,7 @@
         <v>43</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F312" s="1" t="s">
         <v>207</v>
@@ -13120,7 +13119,7 @@
     </row>
     <row r="313" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>203</v>
@@ -13133,7 +13132,7 @@
         <v>44</v>
       </c>
       <c r="E313" s="3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F313" s="3" t="s">
         <v>207</v>
@@ -13147,7 +13146,7 @@
     </row>
     <row r="314" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B314" s="3" t="s">
         <v>203</v>
@@ -13160,7 +13159,7 @@
         <v>44</v>
       </c>
       <c r="E314" s="3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F314" s="3" t="s">
         <v>207</v>
@@ -13187,7 +13186,7 @@
         <v>44</v>
       </c>
       <c r="E315" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F315" s="1" t="s">
         <v>207</v>
@@ -13214,7 +13213,7 @@
         <v>44</v>
       </c>
       <c r="E316" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F316" s="1" t="s">
         <v>207</v>
@@ -13228,7 +13227,7 @@
     </row>
     <row r="317" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B317" s="3" t="s">
         <v>203</v>
@@ -13241,7 +13240,7 @@
         <v>45</v>
       </c>
       <c r="E317" s="3" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F317" s="3" t="s">
         <v>235</v>
@@ -13255,7 +13254,7 @@
     </row>
     <row r="318" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B318" s="3" t="s">
         <v>203</v>
@@ -13268,7 +13267,7 @@
         <v>45</v>
       </c>
       <c r="E318" s="3" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F318" s="3" t="s">
         <v>235</v>
@@ -13282,7 +13281,7 @@
     </row>
     <row r="319" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>203</v>
@@ -13295,7 +13294,7 @@
         <v>47</v>
       </c>
       <c r="E319" s="3" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F319" s="3" t="s">
         <v>207</v>
@@ -13309,7 +13308,7 @@
     </row>
     <row r="320" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>203</v>
@@ -13322,7 +13321,7 @@
         <v>47</v>
       </c>
       <c r="E320" s="3" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F320" s="3" t="s">
         <v>207</v>
@@ -13336,7 +13335,7 @@
     </row>
     <row r="321" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>203</v>
@@ -13363,7 +13362,7 @@
     </row>
     <row r="322" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>203</v>
@@ -13390,7 +13389,7 @@
     </row>
     <row r="323" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B323" s="3" t="s">
         <v>203</v>
@@ -13417,7 +13416,7 @@
     </row>
     <row r="324" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>203</v>
@@ -13444,7 +13443,7 @@
     </row>
     <row r="325" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B325" s="3" t="s">
         <v>203</v>
@@ -13471,7 +13470,7 @@
     </row>
     <row r="326" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B326" s="3" t="s">
         <v>203</v>
@@ -13498,7 +13497,7 @@
     </row>
     <row r="327" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B327" s="3" t="s">
         <v>203</v>
@@ -13511,7 +13510,7 @@
         <v>49</v>
       </c>
       <c r="E327" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F327" s="3" t="s">
         <v>215</v>
@@ -13525,7 +13524,7 @@
     </row>
     <row r="328" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B328" s="3" t="s">
         <v>203</v>
@@ -13538,7 +13537,7 @@
         <v>49</v>
       </c>
       <c r="E328" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F328" s="3" t="s">
         <v>215</v>
@@ -13660,7 +13659,7 @@
     </row>
     <row r="333" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B333" s="3" t="s">
         <v>203</v>
@@ -13673,7 +13672,7 @@
         <v>52</v>
       </c>
       <c r="E333" s="3" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F333" s="3" t="s">
         <v>230</v>
@@ -13700,7 +13699,7 @@
         <v>280</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F334" s="1" t="s">
         <v>230</v>
@@ -13727,7 +13726,7 @@
         <v>281</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F335" s="1" t="s">
         <v>230</v>
@@ -13795,7 +13794,7 @@
     </row>
     <row r="338" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B338" s="3" t="s">
         <v>203</v>
@@ -13808,7 +13807,7 @@
         <v>54</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F338" s="3" t="s">
         <v>207</v>
@@ -13822,7 +13821,7 @@
     </row>
     <row r="339" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B339" s="3" t="s">
         <v>203</v>
@@ -13835,7 +13834,7 @@
         <v>54</v>
       </c>
       <c r="E339" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F339" s="3" t="s">
         <v>207</v>
@@ -13849,7 +13848,7 @@
     </row>
     <row r="340" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B340" s="3" t="s">
         <v>203</v>
@@ -13957,7 +13956,7 @@
     </row>
     <row r="344" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B344" s="3" t="s">
         <v>203</v>
@@ -13984,7 +13983,7 @@
     </row>
     <row r="345" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B345" s="3" t="s">
         <v>203</v>
@@ -13997,7 +13996,7 @@
         <v>57</v>
       </c>
       <c r="E345" s="3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F345" s="3" t="s">
         <v>205</v>
@@ -14011,7 +14010,7 @@
     </row>
     <row r="346" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B346" s="3" t="s">
         <v>203</v>
@@ -14024,7 +14023,7 @@
         <v>57</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F346" s="3" t="s">
         <v>205</v>
@@ -14254,7 +14253,7 @@
     </row>
     <row r="355" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B355" s="3" t="s">
         <v>203</v>
@@ -14281,7 +14280,7 @@
     </row>
     <row r="356" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>203</v>
@@ -14308,7 +14307,7 @@
     </row>
     <row r="357" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>203</v>
@@ -14335,7 +14334,7 @@
     </row>
     <row r="358" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>203</v>
@@ -14362,7 +14361,7 @@
     </row>
     <row r="359" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>203</v>
@@ -14389,7 +14388,7 @@
     </row>
     <row r="360" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>203</v>
@@ -14416,7 +14415,7 @@
     </row>
     <row r="361" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>203</v>
@@ -14443,7 +14442,7 @@
     </row>
     <row r="362" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>203</v>
@@ -14480,10 +14479,10 @@
         <v>5LI</v>
       </c>
       <c r="D363" s="9" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F363" s="1" t="s">
         <v>235</v>
@@ -14507,10 +14506,10 @@
         <v>5LO</v>
       </c>
       <c r="D364" s="9" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F364" s="1" t="s">
         <v>235</v>
@@ -14524,7 +14523,7 @@
     </row>
     <row r="365" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B365" s="3" t="s">
         <v>203</v>
@@ -14534,10 +14533,10 @@
         <v>5RIN</v>
       </c>
       <c r="D365" s="16" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E365" s="3" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F365" s="3" t="s">
         <v>207</v>
@@ -14551,7 +14550,7 @@
     </row>
     <row r="366" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>203</v>
@@ -14561,10 +14560,10 @@
         <v>5ROUT</v>
       </c>
       <c r="D366" s="16" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E366" s="3" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F366" s="3" t="s">
         <v>207</v>
@@ -14740,7 +14739,7 @@
     </row>
     <row r="373" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B373" s="3" t="s">
         <v>203</v>
@@ -14821,7 +14820,7 @@
     </row>
     <row r="376" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B376" s="3" t="s">
         <v>203</v>
@@ -14834,7 +14833,7 @@
         <v>67</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F376" s="3" t="s">
         <v>230</v>
@@ -14861,7 +14860,7 @@
         <v>67</v>
       </c>
       <c r="E377" s="1" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F377" s="1" t="s">
         <v>230</v>
@@ -14888,7 +14887,7 @@
         <v>67</v>
       </c>
       <c r="E378" s="1" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F378" s="1" t="s">
         <v>230</v>
@@ -14902,7 +14901,7 @@
     </row>
     <row r="379" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B379" s="3" t="s">
         <v>203</v>
@@ -14915,7 +14914,7 @@
         <v>6</v>
       </c>
       <c r="E379" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F379" s="3" t="s">
         <v>235</v>
@@ -14929,7 +14928,7 @@
     </row>
     <row r="380" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B380" s="3" t="s">
         <v>203</v>
@@ -14942,7 +14941,7 @@
         <v>6</v>
       </c>
       <c r="E380" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F380" s="3" t="s">
         <v>235</v>
@@ -14956,7 +14955,7 @@
     </row>
     <row r="381" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B381" s="3" t="s">
         <v>203</v>
@@ -14969,7 +14968,7 @@
         <v>6</v>
       </c>
       <c r="E381" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F381" s="3" t="s">
         <v>235</v>
@@ -15145,7 +15144,7 @@
     </row>
     <row r="388" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B388" s="3" t="s">
         <v>203</v>
@@ -15158,7 +15157,7 @@
         <v>7</v>
       </c>
       <c r="E388" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F388" s="3" t="s">
         <v>234</v>
@@ -15172,7 +15171,7 @@
     </row>
     <row r="389" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B389" s="3" t="s">
         <v>203</v>
@@ -15185,7 +15184,7 @@
         <v>7</v>
       </c>
       <c r="E389" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F389" s="3" t="s">
         <v>234</v>
@@ -15199,7 +15198,7 @@
     </row>
     <row r="390" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B390" s="3" t="s">
         <v>203</v>
@@ -15209,10 +15208,10 @@
         <v>7RIN</v>
       </c>
       <c r="D390" s="16" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E390" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F390" s="3" t="s">
         <v>234</v>
@@ -15226,7 +15225,7 @@
     </row>
     <row r="391" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B391" s="3" t="s">
         <v>203</v>
@@ -15236,10 +15235,10 @@
         <v>7ROUT</v>
       </c>
       <c r="D391" s="16" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E391" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F391" s="3" t="s">
         <v>234</v>
@@ -15253,7 +15252,7 @@
     </row>
     <row r="392" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B392" s="3" t="s">
         <v>203</v>
@@ -15263,10 +15262,10 @@
         <v>7XIN</v>
       </c>
       <c r="D392" s="16" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E392" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F392" s="3" t="s">
         <v>234</v>
@@ -15280,7 +15279,7 @@
     </row>
     <row r="393" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B393" s="3" t="s">
         <v>203</v>
@@ -15290,10 +15289,10 @@
         <v>7XOUT</v>
       </c>
       <c r="D393" s="16" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E393" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F393" s="3" t="s">
         <v>234</v>
@@ -15425,10 +15424,10 @@
         <v>82XI</v>
       </c>
       <c r="D398" s="16" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E398" s="3" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F398" s="3" t="s">
         <v>207</v>
@@ -15452,10 +15451,10 @@
         <v>82XO</v>
       </c>
       <c r="D399" s="16" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E399" s="3" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F399" s="3" t="s">
         <v>207</v>
@@ -15533,10 +15532,10 @@
         <v>83XI</v>
       </c>
       <c r="D402" s="16" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E402" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F402" s="3" t="s">
         <v>207</v>
@@ -15560,10 +15559,10 @@
         <v>83XO</v>
       </c>
       <c r="D403" s="16" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E403" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F403" s="3" t="s">
         <v>207</v>
@@ -15577,7 +15576,7 @@
     </row>
     <row r="404" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B404" s="3" t="s">
         <v>203</v>
@@ -15590,7 +15589,7 @@
         <v>88</v>
       </c>
       <c r="E404" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F404" s="3" t="s">
         <v>207</v>
@@ -15604,7 +15603,7 @@
     </row>
     <row r="405" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B405" s="3" t="s">
         <v>203</v>
@@ -15617,7 +15616,7 @@
         <v>88</v>
       </c>
       <c r="E405" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F405" s="3" t="s">
         <v>207</v>
@@ -15685,7 +15684,7 @@
     </row>
     <row r="408" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B408" s="3" t="s">
         <v>203</v>
@@ -15698,7 +15697,7 @@
         <v>8</v>
       </c>
       <c r="E408" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F408" s="3" t="s">
         <v>217</v>
@@ -15712,7 +15711,7 @@
     </row>
     <row r="409" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B409" s="3" t="s">
         <v>203</v>
@@ -15725,7 +15724,7 @@
         <v>8</v>
       </c>
       <c r="E409" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F409" s="3" t="s">
         <v>217</v>
@@ -15739,7 +15738,7 @@
     </row>
     <row r="410" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B410" s="3" t="s">
         <v>203</v>
@@ -15749,10 +15748,10 @@
         <v>8AXIN</v>
       </c>
       <c r="D410" s="16" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E410" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F410" s="3" t="s">
         <v>217</v>
@@ -15766,7 +15765,7 @@
     </row>
     <row r="411" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B411" s="3" t="s">
         <v>203</v>
@@ -15776,10 +15775,10 @@
         <v>8AXOUT</v>
       </c>
       <c r="D411" s="16" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E411" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F411" s="3" t="s">
         <v>217</v>
@@ -15793,7 +15792,7 @@
     </row>
     <row r="412" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B412" s="3" t="s">
         <v>203</v>
@@ -15803,10 +15802,10 @@
         <v>8BXIN</v>
       </c>
       <c r="D412" s="16" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F412" s="3" t="s">
         <v>217</v>
@@ -15820,7 +15819,7 @@
     </row>
     <row r="413" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B413" s="3" t="s">
         <v>203</v>
@@ -15830,10 +15829,10 @@
         <v>8BXOUT</v>
       </c>
       <c r="D413" s="16" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E413" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F413" s="3" t="s">
         <v>217</v>
@@ -16076,7 +16075,7 @@
         <v>91</v>
       </c>
       <c r="E422" s="3" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F422" s="3" t="s">
         <v>207</v>
@@ -16103,7 +16102,7 @@
         <v>91</v>
       </c>
       <c r="E423" s="3" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F423" s="3" t="s">
         <v>207</v>
@@ -16441,7 +16440,7 @@
     </row>
     <row r="436" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B436" s="3" t="s">
         <v>203</v>
@@ -16468,7 +16467,7 @@
     </row>
     <row r="437" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B437" s="3" t="s">
         <v>203</v>
@@ -16495,7 +16494,7 @@
     </row>
     <row r="438" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A438" s="3" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B438" s="3" t="s">
         <v>203</v>
@@ -16508,7 +16507,7 @@
         <v>9</v>
       </c>
       <c r="E438" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F438" s="3" t="s">
         <v>207</v>
@@ -16522,7 +16521,7 @@
     </row>
     <row r="439" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B439" s="3" t="s">
         <v>203</v>
@@ -16535,7 +16534,7 @@
         <v>9</v>
       </c>
       <c r="E439" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F439" s="3" t="s">
         <v>207</v>
@@ -16559,10 +16558,10 @@
         <v>9LI</v>
       </c>
       <c r="D440" s="9" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E440" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F440" s="1" t="s">
         <v>207</v>
@@ -16586,10 +16585,10 @@
         <v>9LO</v>
       </c>
       <c r="D441" s="9" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E441" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F441" s="1" t="s">
         <v>207</v>
@@ -16778,7 +16777,7 @@
         <v>58</v>
       </c>
       <c r="E448" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F448" s="1" t="s">
         <v>207</v>
@@ -16805,7 +16804,7 @@
         <v>58</v>
       </c>
       <c r="E449" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F449" s="1" t="s">
         <v>207</v>
@@ -16927,7 +16926,7 @@
     </row>
     <row r="454" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A454" s="6" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B454" s="6" t="s">
         <v>203</v>
@@ -16954,7 +16953,7 @@
     </row>
     <row r="455" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A455" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B455" s="4" t="s">
         <v>203</v>
@@ -16981,7 +16980,7 @@
     </row>
     <row r="456" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A456" s="4" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B456" s="4" t="s">
         <v>203</v>
@@ -16994,7 +16993,7 @@
         <v>109</v>
       </c>
       <c r="E456" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F456" s="4" t="s">
         <v>325</v>
@@ -17008,7 +17007,7 @@
     </row>
     <row r="457" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A457" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B457" s="4" t="s">
         <v>203</v>
@@ -17021,7 +17020,7 @@
         <v>109</v>
       </c>
       <c r="E457" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F457" s="4" t="s">
         <v>325</v>
@@ -17035,7 +17034,7 @@
     </row>
     <row r="458" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A458" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B458" s="4" t="s">
         <v>203</v>
@@ -17048,7 +17047,7 @@
         <v>109</v>
       </c>
       <c r="E458" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F458" s="4" t="s">
         <v>325</v>
@@ -17062,7 +17061,7 @@
     </row>
     <row r="459" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A459" s="4" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B459" s="4" t="s">
         <v>203</v>
@@ -17075,7 +17074,7 @@
         <v>109</v>
       </c>
       <c r="E459" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F459" s="4" t="s">
         <v>325</v>
@@ -17089,7 +17088,7 @@
     </row>
     <row r="460" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A460" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B460" s="4" t="s">
         <v>203</v>
@@ -17102,7 +17101,7 @@
         <v>125</v>
       </c>
       <c r="E460" s="4" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F460" s="4" t="s">
         <v>328</v>
@@ -17116,7 +17115,7 @@
     </row>
     <row r="461" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A461" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B461" s="4" t="s">
         <v>203</v>
@@ -17129,7 +17128,7 @@
         <v>125</v>
       </c>
       <c r="E461" s="4" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F461" s="4" t="s">
         <v>328</v>
@@ -17143,7 +17142,7 @@
     </row>
     <row r="462" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A462" s="4" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B462" s="4" t="s">
         <v>203</v>
@@ -17156,7 +17155,7 @@
         <v>125</v>
       </c>
       <c r="E462" s="4" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F462" s="4" t="s">
         <v>328</v>
@@ -17170,7 +17169,7 @@
     </row>
     <row r="463" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A463" s="4" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B463" s="4" t="s">
         <v>203</v>
@@ -17197,7 +17196,7 @@
     </row>
     <row r="464" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A464" s="4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B464" s="4" t="s">
         <v>203</v>
@@ -17224,7 +17223,7 @@
     </row>
     <row r="465" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A465" s="4" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B465" s="4" t="s">
         <v>203</v>
@@ -17251,7 +17250,7 @@
     </row>
     <row r="466" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A466" s="4" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B466" s="4" t="s">
         <v>203</v>
@@ -17278,7 +17277,7 @@
     </row>
     <row r="467" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A467" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B467" s="4" t="s">
         <v>203</v>
@@ -17305,7 +17304,7 @@
     </row>
     <row r="468" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A468" s="4" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B468" s="4" t="s">
         <v>203</v>
@@ -17332,7 +17331,7 @@
     </row>
     <row r="469" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A469" s="4" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B469" s="4" t="s">
         <v>203</v>
@@ -17359,7 +17358,7 @@
     </row>
     <row r="470" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A470" s="4" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B470" s="4" t="s">
         <v>203</v>
@@ -17386,7 +17385,7 @@
     </row>
     <row r="471" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A471" s="4" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B471" s="4" t="s">
         <v>203</v>
@@ -17413,7 +17412,7 @@
     </row>
     <row r="472" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A472" s="4" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B472" s="4" t="s">
         <v>203</v>
@@ -17440,7 +17439,7 @@
     </row>
     <row r="473" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A473" s="4" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B473" s="4" t="s">
         <v>203</v>
@@ -17467,7 +17466,7 @@
     </row>
     <row r="474" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A474" s="4" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B474" s="4" t="s">
         <v>203</v>
@@ -17480,7 +17479,7 @@
         <v>133</v>
       </c>
       <c r="E474" s="4" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F474" s="4" t="s">
         <v>333</v>
@@ -17494,7 +17493,7 @@
     </row>
     <row r="475" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A475" s="4" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B475" s="4" t="s">
         <v>203</v>
@@ -17507,7 +17506,7 @@
         <v>133</v>
       </c>
       <c r="E475" s="4" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F475" s="4" t="s">
         <v>333</v>
@@ -17521,7 +17520,7 @@
     </row>
     <row r="476" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A476" s="4" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B476" s="4" t="s">
         <v>203</v>
@@ -17534,7 +17533,7 @@
         <v>133</v>
       </c>
       <c r="E476" s="4" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F476" s="4" t="s">
         <v>333</v>
@@ -17548,7 +17547,7 @@
     </row>
     <row r="477" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A477" s="4" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B477" s="4" t="s">
         <v>203</v>
@@ -17575,7 +17574,7 @@
     </row>
     <row r="478" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A478" s="4" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B478" s="4" t="s">
         <v>203</v>
@@ -17602,7 +17601,7 @@
     </row>
     <row r="479" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A479" s="4" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B479" s="4" t="s">
         <v>203</v>
@@ -17629,7 +17628,7 @@
     </row>
     <row r="480" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A480" s="4" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B480" s="4" t="s">
         <v>203</v>
@@ -17656,7 +17655,7 @@
     </row>
     <row r="481" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A481" s="4" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B481" s="4" t="s">
         <v>203</v>
@@ -17669,7 +17668,7 @@
         <v>148</v>
       </c>
       <c r="E481" s="4" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F481" s="4" t="s">
         <v>333</v>
@@ -17683,7 +17682,7 @@
     </row>
     <row r="482" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A482" s="4" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B482" s="4" t="s">
         <v>203</v>
@@ -17696,7 +17695,7 @@
         <v>148</v>
       </c>
       <c r="E482" s="4" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F482" s="4" t="s">
         <v>333</v>
@@ -17710,7 +17709,7 @@
     </row>
     <row r="483" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A483" s="4" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B483" s="4" t="s">
         <v>203</v>
@@ -17723,7 +17722,7 @@
         <v>148</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F483" s="4" t="s">
         <v>333</v>
@@ -17737,7 +17736,7 @@
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A484" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B484" s="1" t="s">
         <v>203</v>
@@ -17764,7 +17763,7 @@
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A485" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B485" s="1" t="s">
         <v>203</v>
@@ -17791,7 +17790,7 @@
     </row>
     <row r="486" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A486" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B486" s="1" t="s">
         <v>203</v>
@@ -17818,7 +17817,7 @@
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A487" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B487" s="1" t="s">
         <v>203</v>
@@ -17845,7 +17844,7 @@
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A488" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B488" s="1" t="s">
         <v>203</v>
@@ -17872,7 +17871,7 @@
     </row>
     <row r="489" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A489" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B489" s="1" t="s">
         <v>203</v>
@@ -17899,7 +17898,7 @@
     </row>
     <row r="490" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A490" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B490" s="1" t="s">
         <v>203</v>
@@ -17926,7 +17925,7 @@
     </row>
     <row r="491" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A491" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B491" s="1" t="s">
         <v>203</v>
@@ -17953,83 +17952,83 @@
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A492" s="6" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C492" s="6" t="str">
         <f t="shared" si="14"/>
         <v>A</v>
       </c>
       <c r="D492" s="11" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E492" s="6" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="F492" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G492" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H492" s="6" t="s">
         <v>1073</v>
-      </c>
-      <c r="G492" s="6" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H492" s="6" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B493" s="4" t="s">
         <v>1064</v>
-      </c>
-      <c r="B493" s="4" t="s">
-        <v>1066</v>
       </c>
       <c r="C493" s="1" t="str">
         <f t="shared" si="14"/>
         <v>B</v>
       </c>
       <c r="D493" s="9" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E493" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F493" s="4" t="s">
         <v>1071</v>
       </c>
-      <c r="F493" s="4" t="s">
+      <c r="G493" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H493" s="4" t="s">
         <v>1073</v>
-      </c>
-      <c r="G493" s="4" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H493" s="4" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C494" s="1" t="str">
         <f t="shared" si="14"/>
         <v>C</v>
       </c>
       <c r="D494" s="9" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E494" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F494" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="F494" s="4" t="s">
-        <v>1074</v>
-      </c>
       <c r="G494" s="4" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.2">
@@ -18065,12 +18064,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18088,28 +18087,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -18140,7 +18139,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B3" s="1">
         <v>1134</v>
@@ -18149,7 +18148,7 @@
         <v>963</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -18192,7 +18191,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B5" s="1">
         <v>794</v>
@@ -18201,7 +18200,7 @@
         <v>674</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -18244,7 +18243,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B7" s="1">
         <v>907</v>
@@ -18253,7 +18252,7 @@
         <v>770</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -18270,7 +18269,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B8" s="1">
         <v>804</v>
@@ -18279,7 +18278,7 @@
         <v>683</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -18296,7 +18295,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B9" s="1">
         <v>964</v>
@@ -18305,7 +18304,7 @@
         <v>819</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -18348,7 +18347,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B11" s="1">
         <v>1021</v>
@@ -18357,7 +18356,7 @@
         <v>867</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -18400,7 +18399,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B13" s="1">
         <v>65</v>
@@ -18409,7 +18408,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -18478,7 +18477,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B16" s="1">
         <v>650</v>
@@ -18487,7 +18486,7 @@
         <v>552</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -18504,7 +18503,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B17" s="1">
         <v>450</v>
@@ -18513,7 +18512,7 @@
         <v>382</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -18582,7 +18581,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B20" s="1">
         <v>297</v>
@@ -18591,7 +18590,7 @@
         <v>252</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -18608,7 +18607,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B21" s="1">
         <v>357</v>
@@ -18617,7 +18616,7 @@
         <v>303</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -18634,7 +18633,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B22" s="1">
         <v>476</v>
@@ -18643,7 +18642,7 @@
         <v>404</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -18712,7 +18711,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B25" s="1">
         <v>94</v>
@@ -18721,7 +18720,7 @@
         <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18764,7 +18763,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B27" s="1">
         <v>80</v>
@@ -18773,7 +18772,7 @@
         <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18790,7 +18789,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B28" s="1">
         <v>80</v>
@@ -18799,7 +18798,7 @@
         <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -18868,7 +18867,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B31" s="1">
         <v>45</v>
@@ -18877,7 +18876,7 @@
         <v>38</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -18946,7 +18945,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B34" s="1">
         <v>63</v>
@@ -18955,7 +18954,7 @@
         <v>53</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -19102,7 +19101,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B40" s="1">
         <v>94</v>
@@ -19111,7 +19110,7 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -19180,7 +19179,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B43" s="1">
         <v>63</v>
@@ -19189,7 +19188,7 @@
         <v>53</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -19206,7 +19205,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B44" s="1">
         <v>800</v>
@@ -19215,7 +19214,7 @@
         <v>680</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -19258,7 +19257,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B46" s="1">
         <v>28</v>
@@ -19267,7 +19266,7 @@
         <v>23</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -19284,7 +19283,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B47" s="1">
         <v>350</v>
@@ -19293,7 +19292,7 @@
         <v>297</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -19310,7 +19309,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B48" s="1">
         <v>1800</v>
@@ -19319,7 +19318,7 @@
         <v>1530</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -19336,7 +19335,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B49" s="1">
         <v>2700</v>
@@ -19345,7 +19344,7 @@
         <v>2295</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -19362,7 +19361,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B50" s="1">
         <v>4500</v>
@@ -19371,7 +19370,7 @@
         <v>3825</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Add VTA lines to transit capacity files
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3602" uniqueCount="1085">
   <si>
     <t>Name</t>
   </si>
@@ -3266,6 +3266,24 @@
   </si>
   <si>
     <t>21_28RS</t>
+  </si>
+  <si>
+    <t>111_LRCCW</t>
+  </si>
+  <si>
+    <t>111_902LRT</t>
+  </si>
+  <si>
+    <t>111_LRTWCC</t>
+  </si>
+  <si>
+    <t>CCW</t>
+  </si>
+  <si>
+    <t>WCC</t>
+  </si>
+  <si>
+    <t>GREEN LINE</t>
   </si>
 </sst>
 </file>
@@ -4879,11 +4897,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H495"/>
+  <dimension ref="A1:H498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E244" sqref="E244"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E494" sqref="E494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17472,7 +17490,7 @@
         <v>203</v>
       </c>
       <c r="C474" s="4" t="str">
-        <f t="shared" ref="C474:C494" si="14">RIGHT($A474,LEN($A474)-FIND("_",$A474))</f>
+        <f t="shared" ref="C474:C497" si="14">RIGHT($A474,LEN($A474)-FIND("_",$A474))</f>
         <v>L</v>
       </c>
       <c r="D474" s="12" t="s">
@@ -17952,108 +17970,189 @@
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A492" s="6" t="s">
-        <v>1061</v>
+        <v>1079</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>1064</v>
+        <v>927</v>
       </c>
       <c r="C492" s="6" t="str">
         <f t="shared" si="14"/>
-        <v>A</v>
+        <v>LRCCW</v>
       </c>
       <c r="D492" s="11" t="s">
-        <v>1065</v>
+        <v>1082</v>
       </c>
       <c r="E492" s="6" t="s">
-        <v>1068</v>
+        <v>1084</v>
       </c>
       <c r="F492" s="6" t="s">
-        <v>1071</v>
+        <v>333</v>
       </c>
       <c r="G492" s="6" t="s">
-        <v>1071</v>
+        <v>333</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>1073</v>
+        <v>333</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
-        <v>1062</v>
-      </c>
-      <c r="B493" s="4" t="s">
-        <v>1064</v>
+        <v>1080</v>
+      </c>
+      <c r="B493" s="6" t="s">
+        <v>927</v>
       </c>
       <c r="C493" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>B</v>
-      </c>
-      <c r="D493" s="9" t="s">
-        <v>1066</v>
+        <v>902LRT</v>
+      </c>
+      <c r="D493" s="9">
+        <v>902</v>
       </c>
       <c r="E493" s="1" t="s">
-        <v>1069</v>
-      </c>
-      <c r="F493" s="4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="G493" s="4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="H493" s="4" t="s">
-        <v>1073</v>
+        <v>1084</v>
+      </c>
+      <c r="F493" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G493" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H493" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B494" s="4" t="s">
-        <v>1064</v>
+        <v>1081</v>
+      </c>
+      <c r="B494" s="6" t="s">
+        <v>927</v>
       </c>
       <c r="C494" s="1" t="str">
         <f t="shared" si="14"/>
+        <v>LRTWCC</v>
+      </c>
+      <c r="D494" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F494" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G494" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H494" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A495" s="6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B495" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C495" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v>A</v>
+      </c>
+      <c r="D495" s="11" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E495" s="6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F495" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G495" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H495" s="6" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A496" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B496" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C496" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>B</v>
+      </c>
+      <c r="D496" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E496" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F496" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G496" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H496" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A497" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B497" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C497" s="1" t="str">
+        <f t="shared" si="14"/>
         <v>C</v>
       </c>
-      <c r="D494" s="9" t="s">
+      <c r="D497" s="9" t="s">
         <v>1067</v>
       </c>
-      <c r="E494" s="1" t="s">
+      <c r="E497" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="F494" s="4" t="s">
+      <c r="F497" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="G494" s="4" t="s">
+      <c r="G497" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="H494" s="4" t="s">
+      <c r="H497" s="4" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A495" s="1" t="s">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B495" s="1" t="s">
+      <c r="B498" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C495" s="1" t="s">
+      <c r="C498" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D495" s="9" t="s">
+      <c r="D498" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E495" s="1" t="s">
+      <c r="E498" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F495" s="1" t="s">
+      <c r="F498" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G495" s="1" t="s">
+      <c r="G498" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H495" s="1" t="s">
+      <c r="H498" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -18068,7 +18167,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add eBART change to capacity files (see previous commit)
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3632" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="1102">
   <si>
     <t>Name</t>
   </si>
@@ -3332,6 +3332,9 @@
   </si>
   <si>
     <t>Ferry small</t>
+  </si>
+  <si>
+    <t>eBart 1 car</t>
   </si>
 </sst>
 </file>
@@ -18097,11 +18100,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19393,13 +19396,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>909</v>
+        <v>1101</v>
       </c>
       <c r="B50" s="1">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="C50" s="1">
-        <v>297</v>
+        <v>170</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>909</v>
@@ -19419,16 +19422,16 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>1061</v>
+        <v>1075</v>
       </c>
       <c r="B51" s="1">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C51" s="1">
-        <v>382.5</v>
+        <v>340</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1099</v>
+        <v>909</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -19440,6 +19443,32 @@
         <v>0</v>
       </c>
       <c r="H51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B52" s="1">
+        <v>450</v>
+      </c>
+      <c r="C52" s="1">
+        <v>382.5</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
One more time - add 5 car BART capacities
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3638" uniqueCount="1104">
   <si>
     <t>Name</t>
   </si>
@@ -3335,6 +3335,12 @@
   </si>
   <si>
     <t>eBart 1 car</t>
+  </si>
+  <si>
+    <t>5 Car BART</t>
+  </si>
+  <si>
+    <t>5 Car BART RENOVATED</t>
   </si>
 </sst>
 </file>
@@ -18100,11 +18106,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18200,16 +18206,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>1102</v>
       </c>
       <c r="B4" s="1">
-        <v>777</v>
+        <v>555</v>
       </c>
       <c r="C4" s="1">
-        <v>660</v>
+        <v>471.75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>1102</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -18226,16 +18232,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1050</v>
+        <v>1103</v>
       </c>
       <c r="B5" s="1">
-        <v>784</v>
+        <v>560</v>
       </c>
       <c r="C5" s="1">
-        <v>666</v>
+        <v>476</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1050</v>
+        <v>1103</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -18252,16 +18258,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
-        <v>888</v>
+        <v>777</v>
       </c>
       <c r="C6" s="1">
-        <v>765</v>
+        <v>660</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -18278,16 +18284,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B7" s="1">
-        <v>900</v>
+        <v>784</v>
       </c>
       <c r="C7" s="1">
-        <v>770</v>
+        <v>666</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -18304,16 +18310,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>1048</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
-        <v>943</v>
+        <v>888</v>
       </c>
       <c r="C8" s="1">
-        <v>802</v>
+        <v>765</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1048</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -18330,16 +18336,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B9" s="1">
-        <v>952</v>
+        <v>900</v>
       </c>
       <c r="C9" s="1">
-        <v>809</v>
+        <v>770</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -18356,16 +18362,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>1048</v>
       </c>
       <c r="B10" s="1">
-        <v>999</v>
+        <v>943</v>
       </c>
       <c r="C10" s="1">
-        <v>849</v>
+        <v>802</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>1048</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -18382,16 +18388,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B11" s="1">
-        <v>1011</v>
+        <v>952</v>
       </c>
       <c r="C11" s="1">
-        <v>859</v>
+        <v>809</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -18408,146 +18414,146 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>173</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
-        <v>50</v>
+        <v>999</v>
       </c>
       <c r="C12" s="1">
-        <v>42</v>
+        <v>849</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>173</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B13" s="1">
-        <v>65</v>
+        <v>1011</v>
       </c>
       <c r="C13" s="1">
-        <v>55</v>
+        <v>859</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="B14" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G14" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H14" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>287</v>
+        <v>1045</v>
       </c>
       <c r="B15" s="1">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>287</v>
+        <v>1045</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="G15" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H15" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>922</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1">
-        <v>650</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1">
-        <v>552</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>922</v>
+        <v>91</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>931</v>
+        <v>287</v>
       </c>
       <c r="B17" s="1">
-        <v>400</v>
-      </c>
-      <c r="C17" s="17">
-        <v>340</v>
+        <v>63</v>
+      </c>
+      <c r="C17" s="1">
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>931</v>
+        <v>287</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -18556,24 +18562,24 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B18" s="17">
-        <v>450</v>
-      </c>
-      <c r="C18" s="17">
-        <v>382.5</v>
+        <v>922</v>
+      </c>
+      <c r="B18" s="1">
+        <v>650</v>
+      </c>
+      <c r="C18" s="1">
+        <v>552</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>931</v>
+        <v>922</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -18590,13 +18596,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>1100</v>
+        <v>931</v>
       </c>
       <c r="B19" s="1">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="C19" s="17">
-        <v>212.5</v>
+        <v>340</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>931</v>
@@ -18616,13 +18622,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B20" s="1">
-        <v>275</v>
+        <v>1070</v>
+      </c>
+      <c r="B20" s="17">
+        <v>450</v>
       </c>
       <c r="C20" s="17">
-        <v>233.75</v>
+        <v>382.5</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>931</v>
@@ -18642,16 +18648,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>328</v>
+        <v>1100</v>
       </c>
       <c r="B21" s="1">
-        <v>119</v>
-      </c>
-      <c r="C21" s="1">
-        <v>101</v>
+        <v>250</v>
+      </c>
+      <c r="C21" s="17">
+        <v>212.5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>328</v>
+        <v>931</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -18660,24 +18666,24 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>333</v>
+        <v>1071</v>
       </c>
       <c r="B22" s="1">
-        <v>238</v>
-      </c>
-      <c r="C22" s="1">
-        <v>202</v>
+        <v>275</v>
+      </c>
+      <c r="C22" s="17">
+        <v>233.75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>333</v>
+        <v>931</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -18686,24 +18692,24 @@
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>1044</v>
+        <v>328</v>
       </c>
       <c r="B23" s="1">
-        <v>298</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1">
-        <v>253</v>
+        <v>101</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1044</v>
+        <v>328</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -18712,24 +18718,24 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H23" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>1043</v>
+        <v>333</v>
       </c>
       <c r="B24" s="1">
-        <v>357</v>
+        <v>238</v>
       </c>
       <c r="C24" s="1">
-        <v>303</v>
+        <v>202</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1043</v>
+        <v>333</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -18738,24 +18744,24 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H24" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B25" s="1">
-        <v>476</v>
+        <v>298</v>
       </c>
       <c r="C25" s="1">
-        <v>404</v>
+        <v>253</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18764,67 +18770,67 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H25" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>265</v>
+        <v>1043</v>
       </c>
       <c r="B26" s="1">
-        <v>94</v>
+        <v>357</v>
       </c>
       <c r="C26" s="1">
-        <v>79</v>
+        <v>303</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>265</v>
+        <v>1043</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H26" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>217</v>
+        <v>1042</v>
       </c>
       <c r="B27" s="1">
-        <v>94</v>
+        <v>476</v>
       </c>
       <c r="C27" s="1">
-        <v>79</v>
+        <v>404</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>217</v>
+        <v>1042</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>0.04</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H27" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1041</v>
+        <v>265</v>
       </c>
       <c r="B28" s="1">
         <v>94</v>
@@ -18833,7 +18839,7 @@
         <v>79</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1041</v>
+        <v>265</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -18842,67 +18848,67 @@
         <v>0.122</v>
       </c>
       <c r="G28" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H28" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B29" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C29" s="1">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="G29" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H29" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B30" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C30" s="1">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="G30" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H30" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>1039</v>
+        <v>224</v>
       </c>
       <c r="B31" s="1">
         <v>80</v>
@@ -18911,7 +18917,7 @@
         <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1039</v>
+        <v>224</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -18920,67 +18926,67 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G31" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H31" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>261</v>
+        <v>1040</v>
       </c>
       <c r="B32" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>261</v>
+        <v>1040</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G32" s="1">
-        <v>6.2E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H32" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>230</v>
+        <v>1039</v>
       </c>
       <c r="B33" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C33" s="1">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>230</v>
+        <v>1039</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G33" s="1">
-        <v>0.05</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H33" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>1038</v>
+        <v>261</v>
       </c>
       <c r="B34" s="1">
         <v>45</v>
@@ -18989,7 +18995,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1038</v>
+        <v>261</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -18998,24 +19004,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G34" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="B35" s="1">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C35" s="1">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -19024,24 +19030,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G35" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H35" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>207</v>
+        <v>1038</v>
       </c>
       <c r="B36" s="1">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>207</v>
+        <v>1038</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -19050,15 +19056,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H36" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>1037</v>
+        <v>205</v>
       </c>
       <c r="B37" s="1">
         <v>63</v>
@@ -19067,7 +19073,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1037</v>
+        <v>205</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -19076,50 +19082,50 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="B38" s="1">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G38" s="1">
         <v>0.05</v>
       </c>
       <c r="H38" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B39" s="1">
+        <v>63</v>
+      </c>
+      <c r="C39" s="1">
         <v>53</v>
       </c>
-      <c r="B39" s="1">
-        <v>60</v>
-      </c>
-      <c r="C39" s="1">
-        <v>51</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>53</v>
+        <v>1037</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -19128,93 +19134,93 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H39" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>325</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>325</v>
+        <v>36</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="G40" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H40" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="B41" s="1">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
       </c>
       <c r="F41" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H41" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>215</v>
+        <v>325</v>
       </c>
       <c r="B42" s="1">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C42" s="1">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>215</v>
+        <v>325</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G42" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H42" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>1036</v>
+        <v>245</v>
       </c>
       <c r="B43" s="1">
         <v>94</v>
@@ -19223,7 +19229,7 @@
         <v>79</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1036</v>
+        <v>245</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -19232,67 +19238,67 @@
         <v>0.122</v>
       </c>
       <c r="G43" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H43" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B44" s="1">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C44" s="1">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G44" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H44" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>235</v>
+        <v>1036</v>
       </c>
       <c r="B45" s="1">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>235</v>
+        <v>1036</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G45" s="1">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H45" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>1035</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1">
         <v>63</v>
@@ -19301,7 +19307,7 @@
         <v>53</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1035</v>
+        <v>234</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -19310,76 +19316,76 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G46" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H46" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>906</v>
+        <v>235</v>
       </c>
       <c r="B47" s="1">
-        <v>800</v>
+        <v>63</v>
       </c>
       <c r="C47" s="1">
-        <v>680</v>
+        <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>906</v>
+        <v>235</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G47" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H47" s="1">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>259</v>
+        <v>1035</v>
       </c>
       <c r="B48" s="1">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C48" s="1">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>259</v>
+        <v>1035</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G48" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H48" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>1034</v>
+        <v>906</v>
       </c>
       <c r="B49" s="1">
-        <v>28</v>
+        <v>800</v>
       </c>
       <c r="C49" s="1">
-        <v>23</v>
+        <v>680</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>1034</v>
+        <v>906</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -19388,24 +19394,24 @@
         <v>0</v>
       </c>
       <c r="G49" s="1">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H49" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>1101</v>
+        <v>259</v>
       </c>
       <c r="B50" s="1">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>909</v>
+        <v>259</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -19414,24 +19420,24 @@
         <v>0</v>
       </c>
       <c r="G50" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H50" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>1075</v>
+        <v>1034</v>
       </c>
       <c r="B51" s="1">
-        <v>400</v>
+        <v>28</v>
       </c>
       <c r="C51" s="1">
-        <v>340</v>
+        <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>909</v>
+        <v>1034</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -19440,24 +19446,24 @@
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H51" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>1061</v>
+        <v>1101</v>
       </c>
       <c r="B52" s="1">
-        <v>450</v>
+        <v>200</v>
       </c>
       <c r="C52" s="1">
-        <v>382.5</v>
+        <v>170</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1099</v>
+        <v>909</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -19469,6 +19475,58 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B53" s="1">
+        <v>400</v>
+      </c>
+      <c r="C53" s="1">
+        <v>340</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B54" s="1">
+        <v>450</v>
+      </c>
+      <c r="C54" s="1">
+        <v>382.5</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add VTA light rail to capacity files
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3638" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1109">
   <si>
     <t>Name</t>
   </si>
@@ -3341,6 +3341,21 @@
   </si>
   <si>
     <t>5 Car BART RENOVATED</t>
+  </si>
+  <si>
+    <t>VTA LRT1</t>
+  </si>
+  <si>
+    <t>VTA LRT3</t>
+  </si>
+  <si>
+    <t>VTA Light Rail 1</t>
+  </si>
+  <si>
+    <t>VTA Light Rail 2</t>
+  </si>
+  <si>
+    <t>VTA Light Rail 3</t>
   </si>
 </sst>
 </file>
@@ -18106,11 +18121,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19530,6 +19545,87 @@
         <v>0</v>
       </c>
     </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B55" s="1">
+        <v>171</v>
+      </c>
+      <c r="C55" s="17">
+        <f t="shared" ref="C55:C57" si="0">B55*0.85</f>
+        <v>145.35</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B56" s="1">
+        <v>342</v>
+      </c>
+      <c r="C56" s="17">
+        <f t="shared" si="0"/>
+        <v>290.7</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H56" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B57" s="1">
+        <v>513</v>
+      </c>
+      <c r="C57" s="17">
+        <f t="shared" si="0"/>
+        <v>436.05</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H57" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add missing transit capacity types
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
@@ -17,19 +17,11 @@
     <sheet name="transitVehicleToCapacity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="1111">
   <si>
     <t>Name</t>
   </si>
@@ -3356,6 +3348,12 @@
   </si>
   <si>
     <t>VTA Light Rail 3</t>
+  </si>
+  <si>
+    <t>Airport Tram</t>
+  </si>
+  <si>
+    <t>SMART 2 Car Train</t>
   </si>
 </sst>
 </file>
@@ -3876,7 +3874,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3911,6 +3909,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4234,9 +4236,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18121,11 +18123,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19626,6 +19628,58 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B58" s="18">
+        <v>89</v>
+      </c>
+      <c r="C58" s="19">
+        <v>75.649999999999991</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B59" s="20">
+        <v>318</v>
+      </c>
+      <c r="C59" s="21">
+        <v>270.3</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E59" s="20">
+        <v>0</v>
+      </c>
+      <c r="F59" s="20">
+        <v>0</v>
+      </c>
+      <c r="G59" s="20">
+        <v>0</v>
+      </c>
+      <c r="H59" s="20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Change to eBART mode (from 136 to 122)
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2756,9 +2756,6 @@
     <t>EBART</t>
   </si>
   <si>
-    <t>136_</t>
-  </si>
-  <si>
     <t>SMART</t>
   </si>
   <si>
@@ -3354,6 +3351,9 @@
   </si>
   <si>
     <t>SMART 2 Car Train</t>
+  </si>
+  <si>
+    <t>122_</t>
   </si>
 </sst>
 </file>
@@ -3958,8 +3958,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4238,7 +4266,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4251,87 +4279,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C4" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C5" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B8" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C8" t="s">
         <v>205</v>
@@ -4339,10 +4367,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C9" t="s">
         <v>333</v>
@@ -4350,21 +4378,21 @@
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B10" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C10" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C11" t="s">
         <v>261</v>
@@ -4372,7 +4400,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -4383,54 +4411,54 @@
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B13" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C13" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1027</v>
+        <v>1110</v>
       </c>
       <c r="B14" t="s">
-        <v>1026</v>
+        <v>910</v>
       </c>
       <c r="C14" t="s">
-        <v>261</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>923</v>
+        <v>1026</v>
       </c>
       <c r="B15" t="s">
-        <v>922</v>
+        <v>1025</v>
       </c>
       <c r="C15" t="s">
-        <v>922</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>922</v>
+      </c>
+      <c r="B16" t="s">
         <v>921</v>
       </c>
-      <c r="B16" t="s">
-        <v>920</v>
-      </c>
       <c r="C16" t="s">
-        <v>906</v>
+        <v>921</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>920</v>
+      </c>
+      <c r="B17" t="s">
         <v>919</v>
-      </c>
-      <c r="B17" t="s">
-        <v>918</v>
       </c>
       <c r="C17" t="s">
         <v>906</v>
@@ -4438,10 +4466,10 @@
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>918</v>
+      </c>
+      <c r="B18" t="s">
         <v>917</v>
-      </c>
-      <c r="B18" t="s">
-        <v>916</v>
       </c>
       <c r="C18" t="s">
         <v>906</v>
@@ -4449,35 +4477,35 @@
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>916</v>
+      </c>
+      <c r="B19" t="s">
         <v>915</v>
       </c>
-      <c r="B19" t="s">
-        <v>914</v>
-      </c>
       <c r="C19" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>914</v>
+      </c>
+      <c r="B20" t="s">
         <v>913</v>
       </c>
-      <c r="B20" t="s">
-        <v>912</v>
-      </c>
       <c r="C20" t="s">
-        <v>1074</v>
+        <v>913</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>912</v>
+      </c>
+      <c r="B21" t="s">
         <v>911</v>
       </c>
-      <c r="B21" t="s">
-        <v>910</v>
-      </c>
       <c r="C21" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -4488,15 +4516,15 @@
         <v>907</v>
       </c>
       <c r="C22" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B23" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C23" t="s">
         <v>261</v>
@@ -4504,10 +4532,10 @@
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B24" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C24" t="s">
         <v>261</v>
@@ -4515,10 +4543,10 @@
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B25" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C25" t="s">
         <v>261</v>
@@ -4526,10 +4554,10 @@
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B26" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C26" t="s">
         <v>261</v>
@@ -4537,10 +4565,10 @@
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B27" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C27" t="s">
         <v>261</v>
@@ -4548,10 +4576,10 @@
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B28" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C28" t="s">
         <v>261</v>
@@ -4559,10 +4587,10 @@
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B29" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C29" t="s">
         <v>261</v>
@@ -4570,10 +4598,10 @@
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B30" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C30" t="s">
         <v>287</v>
@@ -4581,10 +4609,10 @@
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B31" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C31" t="s">
         <v>205</v>
@@ -4592,10 +4620,10 @@
     </row>
     <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B32" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C32" t="s">
         <v>205</v>
@@ -4603,10 +4631,10 @@
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B33" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C33" t="s">
         <v>205</v>
@@ -4614,10 +4642,10 @@
     </row>
     <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B34" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C34" t="s">
         <v>205</v>
@@ -4625,10 +4653,10 @@
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B35" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C35" t="s">
         <v>205</v>
@@ -4636,10 +4664,10 @@
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B36" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C36" t="s">
         <v>205</v>
@@ -4647,10 +4675,10 @@
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B37" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C37" t="s">
         <v>205</v>
@@ -4658,10 +4686,10 @@
     </row>
     <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B38" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C38" t="s">
         <v>205</v>
@@ -4669,10 +4697,10 @@
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B39" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C39" t="s">
         <v>205</v>
@@ -4680,10 +4708,10 @@
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B40" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C40" t="s">
         <v>205</v>
@@ -4691,10 +4719,10 @@
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B41" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C41" t="s">
         <v>205</v>
@@ -4702,10 +4730,10 @@
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B42" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C42" t="s">
         <v>205</v>
@@ -4713,10 +4741,10 @@
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B43" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C43" t="s">
         <v>205</v>
@@ -4724,10 +4752,10 @@
     </row>
     <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B44" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C44" t="s">
         <v>205</v>
@@ -4735,10 +4763,10 @@
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B45" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C45" t="s">
         <v>205</v>
@@ -4746,10 +4774,10 @@
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B46" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C46" t="s">
         <v>205</v>
@@ -4757,10 +4785,10 @@
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B47" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C47" t="s">
         <v>205</v>
@@ -4768,10 +4796,10 @@
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B48" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C48" t="s">
         <v>205</v>
@@ -4779,10 +4807,10 @@
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B49" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C49" t="s">
         <v>205</v>
@@ -4790,10 +4818,10 @@
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B50" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C50" t="s">
         <v>205</v>
@@ -4801,10 +4829,10 @@
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B51" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C51" t="s">
         <v>205</v>
@@ -4812,10 +4840,10 @@
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B52" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C52" t="s">
         <v>205</v>
@@ -4823,10 +4851,10 @@
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B53" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C53" t="s">
         <v>205</v>
@@ -4834,10 +4862,10 @@
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B54" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C54" t="s">
         <v>205</v>
@@ -4845,10 +4873,10 @@
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B55" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C55" t="s">
         <v>205</v>
@@ -4856,10 +4884,10 @@
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B56" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C56" t="s">
         <v>205</v>
@@ -4867,10 +4895,10 @@
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B57" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C57" t="s">
         <v>205</v>
@@ -4878,10 +4906,10 @@
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B58" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C58" t="s">
         <v>205</v>
@@ -4889,10 +4917,10 @@
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B59" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C59" t="s">
         <v>205</v>
@@ -4900,10 +4928,10 @@
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B60" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C60" t="s">
         <v>205</v>
@@ -4911,10 +4939,10 @@
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B61" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C61" t="s">
         <v>205</v>
@@ -4922,10 +4950,10 @@
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B62" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C62" t="s">
         <v>205</v>
@@ -4933,10 +4961,10 @@
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B63" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C63" t="s">
         <v>205</v>
@@ -4944,10 +4972,10 @@
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B64" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C64" t="s">
         <v>205</v>
@@ -4955,10 +4983,10 @@
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B65" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C65" t="s">
         <v>205</v>
@@ -4966,13 +4994,13 @@
     </row>
     <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
   </sheetData>
@@ -5091,10 +5119,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>23</v>
@@ -5117,10 +5145,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -5143,10 +5171,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>27</v>
@@ -5169,10 +5197,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>27</v>
@@ -5195,10 +5223,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>29</v>
@@ -5221,10 +5249,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>29</v>
@@ -5241,16 +5269,16 @@
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -5267,16 +5295,16 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -5299,10 +5327,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>31</v>
@@ -5325,10 +5353,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>31</v>
@@ -5351,10 +5379,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>31</v>
@@ -5377,10 +5405,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>31</v>
@@ -5403,10 +5431,10 @@
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>31</v>
@@ -5429,10 +5457,10 @@
         <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>31</v>
@@ -5455,10 +5483,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>31</v>
@@ -5481,10 +5509,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>31</v>
@@ -5507,10 +5535,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>31</v>
@@ -5533,10 +5561,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>31</v>
@@ -5559,10 +5587,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>31</v>
@@ -5585,10 +5613,10 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>31</v>
@@ -5611,10 +5639,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>31</v>
@@ -5637,10 +5665,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>31</v>
@@ -5663,10 +5691,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>31</v>
@@ -11152,7 +11180,7 @@
     </row>
     <row r="238" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>203</v>
@@ -11179,7 +11207,7 @@
     </row>
     <row r="239" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>203</v>
@@ -18010,37 +18038,37 @@
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A492" s="6" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C492" s="6" t="str">
         <f t="shared" si="12"/>
         <v>LRCCW</v>
       </c>
       <c r="D492" s="11" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E492" s="6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F492" s="6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G492" s="6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C493" s="1" t="str">
         <f t="shared" si="12"/>
@@ -18050,43 +18078,43 @@
         <v>902</v>
       </c>
       <c r="E493" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C494" s="1" t="str">
         <f t="shared" si="12"/>
         <v>LRTWCC</v>
       </c>
       <c r="D494" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E494" s="1" t="s">
         <v>1068</v>
       </c>
-      <c r="E494" s="1" t="s">
-        <v>1069</v>
-      </c>
       <c r="F494" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.2">
@@ -18145,28 +18173,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -18197,7 +18225,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B3" s="1">
         <v>1200</v>
@@ -18206,7 +18234,7 @@
         <v>1020</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -18223,7 +18251,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B4" s="1">
         <v>555</v>
@@ -18232,7 +18260,7 @@
         <v>471.75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -18249,7 +18277,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B5" s="1">
         <v>560</v>
@@ -18258,7 +18286,7 @@
         <v>476</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -18301,7 +18329,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B7" s="1">
         <v>784</v>
@@ -18310,7 +18338,7 @@
         <v>666</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -18353,7 +18381,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B9" s="1">
         <v>900</v>
@@ -18362,7 +18390,7 @@
         <v>770</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -18379,7 +18407,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B10" s="1">
         <v>943</v>
@@ -18388,7 +18416,7 @@
         <v>802</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -18405,7 +18433,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B11" s="1">
         <v>952</v>
@@ -18414,7 +18442,7 @@
         <v>809</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -18457,7 +18485,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B13" s="1">
         <v>1011</v>
@@ -18466,7 +18494,7 @@
         <v>859</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -18509,7 +18537,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B15" s="1">
         <v>65</v>
@@ -18518,7 +18546,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -18587,7 +18615,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B18" s="1">
         <v>650</v>
@@ -18596,7 +18624,7 @@
         <v>552</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -18613,7 +18641,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B19" s="1">
         <v>400</v>
@@ -18622,7 +18650,7 @@
         <v>340</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -18639,7 +18667,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B20" s="17">
         <v>450</v>
@@ -18648,7 +18676,7 @@
         <v>382.5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -18665,7 +18693,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B21" s="1">
         <v>250</v>
@@ -18674,7 +18702,7 @@
         <v>212.5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -18691,7 +18719,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B22" s="1">
         <v>275</v>
@@ -18700,7 +18728,7 @@
         <v>233.75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -18769,7 +18797,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B25" s="1">
         <v>298</v>
@@ -18778,7 +18806,7 @@
         <v>253</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18795,7 +18823,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B26" s="1">
         <v>357</v>
@@ -18804,7 +18832,7 @@
         <v>303</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -18821,7 +18849,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B27" s="1">
         <v>476</v>
@@ -18830,7 +18858,7 @@
         <v>404</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18899,7 +18927,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B30" s="1">
         <v>94</v>
@@ -18908,7 +18936,7 @@
         <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -18951,7 +18979,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B32" s="1">
         <v>80</v>
@@ -18960,7 +18988,7 @@
         <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -18977,7 +19005,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B33" s="1">
         <v>80</v>
@@ -18986,7 +19014,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -19055,7 +19083,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B36" s="1">
         <v>45</v>
@@ -19064,7 +19092,7 @@
         <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -19133,7 +19161,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B39" s="1">
         <v>63</v>
@@ -19142,7 +19170,7 @@
         <v>53</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -19289,7 +19317,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B45" s="1">
         <v>94</v>
@@ -19298,7 +19326,7 @@
         <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -19367,7 +19395,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B48" s="1">
         <v>63</v>
@@ -19376,7 +19404,7 @@
         <v>53</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -19445,7 +19473,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B51" s="1">
         <v>28</v>
@@ -19454,7 +19482,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -19471,7 +19499,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B52" s="1">
         <v>200</v>
@@ -19497,7 +19525,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B53" s="1">
         <v>400</v>
@@ -19523,7 +19551,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B54" s="1">
         <v>450</v>
@@ -19532,7 +19560,7 @@
         <v>382.5</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -19549,7 +19577,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B55" s="1">
         <v>171</v>
@@ -19559,7 +19587,7 @@
         <v>145.35</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -19576,7 +19604,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B56" s="1">
         <v>342</v>
@@ -19586,7 +19614,7 @@
         <v>290.7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -19603,7 +19631,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B57" s="1">
         <v>513</v>
@@ -19613,7 +19641,7 @@
         <v>436.05</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -19630,7 +19658,7 @@
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B58" s="18">
         <v>89</v>
@@ -19639,7 +19667,7 @@
         <v>75.649999999999991</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -19656,7 +19684,7 @@
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B59" s="20">
         <v>318</v>
@@ -19665,7 +19693,7 @@
         <v>270.3</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E59" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
fix BART 10 car capacities
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\TM1_2015_Base_Network\trn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
@@ -4264,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -18153,9 +18153,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18202,10 +18202,10 @@
         <v>26</v>
       </c>
       <c r="B2" s="1">
-        <v>1100</v>
+        <v>1110</v>
       </c>
       <c r="C2" s="1">
-        <v>935</v>
+        <v>943.5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -18228,10 +18228,10 @@
         <v>1050</v>
       </c>
       <c r="B3" s="1">
-        <v>1200</v>
+        <v>1120</v>
       </c>
       <c r="C3" s="1">
-        <v>1020</v>
+        <v>952</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1050</v>

</xml_diff>

<commit_message>
add new Caltrain capacities
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3652" uniqueCount="1113">
   <si>
     <t>Name</t>
   </si>
@@ -3354,6 +3354,12 @@
   </si>
   <si>
     <t>122_</t>
+  </si>
+  <si>
+    <t>Caltrain PCEP</t>
+  </si>
+  <si>
+    <t>Caltrain PCBB</t>
   </si>
 </sst>
 </file>
@@ -18151,11 +18157,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13:C13"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18618,10 +18624,10 @@
         <v>921</v>
       </c>
       <c r="B18" s="1">
-        <v>650</v>
+        <v>1444</v>
       </c>
       <c r="C18" s="1">
-        <v>552</v>
+        <v>1228</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>921</v>
@@ -18641,16 +18647,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>930</v>
+        <v>1111</v>
       </c>
       <c r="B19" s="1">
-        <v>400</v>
-      </c>
-      <c r="C19" s="17">
-        <v>340</v>
+        <v>1502</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1276.7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -18667,16 +18673,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B20" s="17">
-        <v>450</v>
-      </c>
-      <c r="C20" s="17">
-        <v>382.5</v>
+        <v>1112</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1841</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1564.85</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>930</v>
+        <v>921</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -18693,13 +18699,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>1099</v>
+        <v>930</v>
       </c>
       <c r="B21" s="1">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="C21" s="17">
-        <v>212.5</v>
+        <v>340</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>930</v>
@@ -18719,13 +18725,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B22" s="1">
-        <v>275</v>
+        <v>1069</v>
+      </c>
+      <c r="B22" s="17">
+        <v>450</v>
       </c>
       <c r="C22" s="17">
-        <v>233.75</v>
+        <v>382.5</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>930</v>
@@ -18745,16 +18751,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>328</v>
+        <v>1099</v>
       </c>
       <c r="B23" s="1">
-        <v>119</v>
-      </c>
-      <c r="C23" s="1">
-        <v>101</v>
+        <v>250</v>
+      </c>
+      <c r="C23" s="17">
+        <v>212.5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>328</v>
+        <v>930</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -18763,24 +18769,24 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>333</v>
+        <v>1070</v>
       </c>
       <c r="B24" s="1">
-        <v>238</v>
-      </c>
-      <c r="C24" s="1">
-        <v>202</v>
+        <v>275</v>
+      </c>
+      <c r="C24" s="17">
+        <v>233.75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>333</v>
+        <v>930</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -18789,24 +18795,24 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1043</v>
+        <v>328</v>
       </c>
       <c r="B25" s="1">
-        <v>298</v>
+        <v>119</v>
       </c>
       <c r="C25" s="1">
-        <v>253</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1043</v>
+        <v>328</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18815,24 +18821,24 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H25" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>1042</v>
+        <v>333</v>
       </c>
       <c r="B26" s="1">
-        <v>357</v>
+        <v>238</v>
       </c>
       <c r="C26" s="1">
-        <v>303</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1042</v>
+        <v>333</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -18841,24 +18847,24 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H26" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="B27" s="1">
-        <v>476</v>
+        <v>298</v>
       </c>
       <c r="C27" s="1">
-        <v>404</v>
+        <v>253</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18867,67 +18873,67 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H27" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>265</v>
+        <v>1042</v>
       </c>
       <c r="B28" s="1">
-        <v>94</v>
+        <v>357</v>
       </c>
       <c r="C28" s="1">
-        <v>79</v>
+        <v>303</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>265</v>
+        <v>1042</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H28" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>217</v>
+        <v>1041</v>
       </c>
       <c r="B29" s="1">
-        <v>94</v>
+        <v>476</v>
       </c>
       <c r="C29" s="1">
-        <v>79</v>
+        <v>404</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>217</v>
+        <v>1041</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>0.04</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H29" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>1040</v>
+        <v>265</v>
       </c>
       <c r="B30" s="1">
         <v>94</v>
@@ -18936,7 +18942,7 @@
         <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1040</v>
+        <v>265</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -18945,67 +18951,67 @@
         <v>0.122</v>
       </c>
       <c r="G30" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H30" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="G31" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H31" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B32" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C32" s="1">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="G32" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H32" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>1038</v>
+        <v>224</v>
       </c>
       <c r="B33" s="1">
         <v>80</v>
@@ -19014,7 +19020,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1038</v>
+        <v>224</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -19023,67 +19029,67 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G33" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H33" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>261</v>
+        <v>1039</v>
       </c>
       <c r="B34" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>261</v>
+        <v>1039</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>6.2E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>230</v>
+        <v>1038</v>
       </c>
       <c r="B35" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C35" s="1">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>230</v>
+        <v>1038</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G35" s="1">
-        <v>0.05</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H35" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>1037</v>
+        <v>261</v>
       </c>
       <c r="B36" s="1">
         <v>45</v>
@@ -19092,7 +19098,7 @@
         <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1037</v>
+        <v>261</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -19101,24 +19107,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="B37" s="1">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -19127,24 +19133,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H37" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>207</v>
+        <v>1037</v>
       </c>
       <c r="B38" s="1">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>207</v>
+        <v>1037</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -19153,15 +19159,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H38" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>1036</v>
+        <v>205</v>
       </c>
       <c r="B39" s="1">
         <v>63</v>
@@ -19170,7 +19176,7 @@
         <v>53</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1036</v>
+        <v>205</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -19179,50 +19185,50 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="B40" s="1">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G40" s="1">
         <v>0.05</v>
       </c>
       <c r="H40" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B41" s="1">
+        <v>63</v>
+      </c>
+      <c r="C41" s="1">
         <v>53</v>
       </c>
-      <c r="B41" s="1">
-        <v>60</v>
-      </c>
-      <c r="C41" s="1">
-        <v>51</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>1036</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -19231,93 +19237,93 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H41" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>325</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>325</v>
+        <v>36</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="G42" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H42" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="B43" s="1">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H43" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>215</v>
+        <v>325</v>
       </c>
       <c r="B44" s="1">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C44" s="1">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>215</v>
+        <v>325</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H44" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>1035</v>
+        <v>245</v>
       </c>
       <c r="B45" s="1">
         <v>94</v>
@@ -19326,7 +19332,7 @@
         <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1035</v>
+        <v>245</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -19335,67 +19341,67 @@
         <v>0.122</v>
       </c>
       <c r="G45" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H45" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B46" s="1">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C46" s="1">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G46" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H46" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>235</v>
+        <v>1035</v>
       </c>
       <c r="B47" s="1">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C47" s="1">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>235</v>
+        <v>1035</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G47" s="1">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H47" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>1034</v>
+        <v>234</v>
       </c>
       <c r="B48" s="1">
         <v>63</v>
@@ -19404,7 +19410,7 @@
         <v>53</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1034</v>
+        <v>234</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -19413,76 +19419,76 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G48" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H48" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>906</v>
+        <v>235</v>
       </c>
       <c r="B49" s="1">
-        <v>800</v>
+        <v>63</v>
       </c>
       <c r="C49" s="1">
-        <v>680</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>906</v>
+        <v>235</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G49" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H49" s="1">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>259</v>
+        <v>1034</v>
       </c>
       <c r="B50" s="1">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C50" s="1">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>259</v>
+        <v>1034</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G50" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H50" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>1033</v>
+        <v>906</v>
       </c>
       <c r="B51" s="1">
-        <v>28</v>
+        <v>800</v>
       </c>
       <c r="C51" s="1">
-        <v>23</v>
+        <v>680</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1033</v>
+        <v>906</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -19491,24 +19497,24 @@
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>1100</v>
+        <v>259</v>
       </c>
       <c r="B52" s="1">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>909</v>
+        <v>259</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -19517,24 +19523,24 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>1074</v>
+        <v>1033</v>
       </c>
       <c r="B53" s="1">
-        <v>400</v>
+        <v>28</v>
       </c>
       <c r="C53" s="1">
-        <v>340</v>
+        <v>23</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>909</v>
+        <v>1033</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -19543,24 +19549,24 @@
         <v>0</v>
       </c>
       <c r="G53" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H53" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1060</v>
+        <v>1100</v>
       </c>
       <c r="B54" s="1">
-        <v>450</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1">
-        <v>382.5</v>
+        <v>170</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1098</v>
+        <v>909</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -19577,17 +19583,16 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1103</v>
+        <v>1074</v>
       </c>
       <c r="B55" s="1">
-        <v>171</v>
-      </c>
-      <c r="C55" s="17">
-        <f t="shared" ref="C55:C57" si="0">B55*0.85</f>
-        <v>145.35</v>
+        <v>400</v>
+      </c>
+      <c r="C55" s="1">
+        <v>340</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1105</v>
+        <v>909</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -19596,115 +19601,168 @@
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H55" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B56" s="1">
+        <v>450</v>
+      </c>
+      <c r="C56" s="1">
+        <v>382.5</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B57" s="1">
+        <v>171</v>
+      </c>
+      <c r="C57" s="17">
+        <f t="shared" ref="C57:C59" si="0">B57*0.85</f>
+        <v>145.35</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>1071</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B58" s="1">
         <v>342</v>
       </c>
-      <c r="C56" s="17">
+      <c r="C58" s="17">
         <f t="shared" si="0"/>
         <v>290.7</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>1106</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E58" s="1">
         <v>0</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F58" s="1">
         <v>0</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G58" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H58" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>1104</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B59" s="1">
         <v>513</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C59" s="17">
         <f t="shared" si="0"/>
         <v>436.05</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>1107</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E59" s="1">
         <v>0</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F59" s="1">
         <v>0</v>
       </c>
-      <c r="G57" s="1">
+      <c r="G59" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H59" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
         <v>1072</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B60" s="18">
         <v>89</v>
       </c>
-      <c r="C58" s="19">
+      <c r="C60" s="19">
         <v>75.649999999999991</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D60" s="18" t="s">
         <v>1108</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E60" s="1">
         <v>0</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F60" s="1">
         <v>0</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G60" s="1">
         <v>0</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H60" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>1073</v>
       </c>
-      <c r="B59" s="20">
+      <c r="B61" s="20">
         <v>318</v>
       </c>
-      <c r="C59" s="21">
+      <c r="C61" s="21">
         <v>270.3</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D61" s="20" t="s">
         <v>1109</v>
       </c>
-      <c r="E59" s="20">
+      <c r="E61" s="20">
         <v>0</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F61" s="20">
         <v>0</v>
       </c>
-      <c r="G59" s="20">
+      <c r="G61" s="20">
         <v>0</v>
       </c>
-      <c r="H59" s="20">
+      <c r="H61" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change eBART mode to 120
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3659" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3656" uniqueCount="1114">
   <si>
     <t>Name</t>
   </si>
@@ -2753,9 +2753,6 @@
     <t>eBart</t>
   </si>
   <si>
-    <t>EBART</t>
-  </si>
-  <si>
     <t>SMART</t>
   </si>
   <si>
@@ -3353,22 +3350,19 @@
     <t>SMART 2 Car Train</t>
   </si>
   <si>
-    <t>122_</t>
-  </si>
-  <si>
     <t>Caltrain PCEP</t>
   </si>
   <si>
     <t>Caltrain PCBB</t>
   </si>
   <si>
-    <t>122_EBART</t>
-  </si>
-  <si>
     <t>eBART</t>
   </si>
   <si>
     <t>BART Yellow line extension</t>
+  </si>
+  <si>
+    <t>120_EBART</t>
   </si>
 </sst>
 </file>
@@ -4277,11 +4271,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4294,87 +4288,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C5" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C6" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C7" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B8" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C8" t="s">
         <v>205</v>
@@ -4382,10 +4376,10 @@
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B9" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C9" t="s">
         <v>333</v>
@@ -4393,21 +4387,21 @@
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B10" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C10" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B11" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C11" t="s">
         <v>261</v>
@@ -4415,7 +4409,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -4426,54 +4420,54 @@
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B13" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1110</v>
+        <v>1025</v>
       </c>
       <c r="B14" t="s">
-        <v>910</v>
+        <v>1024</v>
       </c>
       <c r="C14" t="s">
-        <v>1074</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1026</v>
+        <v>921</v>
       </c>
       <c r="B15" t="s">
-        <v>1025</v>
+        <v>920</v>
       </c>
       <c r="C15" t="s">
-        <v>261</v>
+        <v>920</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B16" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="C16" t="s">
-        <v>921</v>
+        <v>906</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="B17" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C17" t="s">
         <v>906</v>
@@ -4481,10 +4475,10 @@
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="B18" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="C18" t="s">
         <v>906</v>
@@ -4492,54 +4486,54 @@
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="B19" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C19" t="s">
-        <v>906</v>
+        <v>912</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="B20" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="C20" t="s">
-        <v>913</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="B21" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="C21" t="s">
-        <v>1073</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>908</v>
+        <v>1023</v>
       </c>
       <c r="B22" t="s">
-        <v>907</v>
+        <v>1022</v>
       </c>
       <c r="C22" t="s">
-        <v>1060</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B23" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="C23" t="s">
         <v>261</v>
@@ -4547,10 +4541,10 @@
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="B24" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="C24" t="s">
         <v>261</v>
@@ -4558,10 +4552,10 @@
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B25" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C25" t="s">
         <v>261</v>
@@ -4569,10 +4563,10 @@
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B26" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C26" t="s">
         <v>261</v>
@@ -4580,10 +4574,10 @@
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B27" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="C27" t="s">
         <v>261</v>
@@ -4591,10 +4585,10 @@
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B28" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="C28" t="s">
         <v>261</v>
@@ -4602,32 +4596,32 @@
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="B29" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="C29" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B30" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="C30" t="s">
-        <v>287</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B31" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C31" t="s">
         <v>205</v>
@@ -4635,10 +4629,10 @@
     </row>
     <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="B32" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="C32" t="s">
         <v>205</v>
@@ -4646,10 +4640,10 @@
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="B33" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="C33" t="s">
         <v>205</v>
@@ -4657,10 +4651,10 @@
     </row>
     <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="B34" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C34" t="s">
         <v>205</v>
@@ -4668,10 +4662,10 @@
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B35" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="C35" t="s">
         <v>205</v>
@@ -4679,10 +4673,10 @@
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B36" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="C36" t="s">
         <v>205</v>
@@ -4690,10 +4684,10 @@
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="B37" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="C37" t="s">
         <v>205</v>
@@ -4701,10 +4695,10 @@
     </row>
     <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B38" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="C38" t="s">
         <v>205</v>
@@ -4712,10 +4706,10 @@
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B39" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="C39" t="s">
         <v>205</v>
@@ -4723,10 +4717,10 @@
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B40" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="C40" t="s">
         <v>205</v>
@@ -4734,10 +4728,10 @@
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B41" t="s">
-        <v>987</v>
+        <v>979</v>
       </c>
       <c r="C41" t="s">
         <v>205</v>
@@ -4745,10 +4739,10 @@
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B42" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="C42" t="s">
         <v>205</v>
@@ -4756,10 +4750,10 @@
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="B43" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="C43" t="s">
         <v>205</v>
@@ -4767,10 +4761,10 @@
     </row>
     <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B44" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="C44" t="s">
         <v>205</v>
@@ -4778,10 +4772,10 @@
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B45" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C45" t="s">
         <v>205</v>
@@ -4789,10 +4783,10 @@
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="B46" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C46" t="s">
         <v>205</v>
@@ -4800,10 +4794,10 @@
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B47" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="C47" t="s">
         <v>205</v>
@@ -4811,10 +4805,10 @@
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="B48" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="C48" t="s">
         <v>205</v>
@@ -4822,10 +4816,10 @@
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="B49" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="C49" t="s">
         <v>205</v>
@@ -4833,10 +4827,10 @@
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B50" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C50" t="s">
         <v>205</v>
@@ -4844,10 +4838,10 @@
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B51" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="C51" t="s">
         <v>205</v>
@@ -4855,10 +4849,10 @@
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B52" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="C52" t="s">
         <v>205</v>
@@ -4866,10 +4860,10 @@
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B53" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="C53" t="s">
         <v>205</v>
@@ -4877,10 +4871,10 @@
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="B54" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="C54" t="s">
         <v>205</v>
@@ -4888,10 +4882,10 @@
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B55" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C55" t="s">
         <v>205</v>
@@ -4899,10 +4893,10 @@
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B56" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="C56" t="s">
         <v>205</v>
@@ -4910,10 +4904,10 @@
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="B57" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="C57" t="s">
         <v>205</v>
@@ -4921,10 +4915,10 @@
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B58" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C58" t="s">
         <v>205</v>
@@ -4932,10 +4926,10 @@
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="B59" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="C59" t="s">
         <v>205</v>
@@ -4943,10 +4937,10 @@
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="B60" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C60" t="s">
         <v>205</v>
@@ -4954,10 +4948,10 @@
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="B61" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="C61" t="s">
         <v>205</v>
@@ -4965,10 +4959,10 @@
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="B62" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
       <c r="C62" t="s">
         <v>205</v>
@@ -4976,10 +4970,10 @@
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B63" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C63" t="s">
         <v>205</v>
@@ -4987,10 +4981,10 @@
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="B64" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="C64" t="s">
         <v>205</v>
@@ -4998,24 +4992,13 @@
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>944</v>
+        <v>1031</v>
       </c>
       <c r="B65" t="s">
-        <v>943</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
   </sheetData>
@@ -5028,9 +5011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H496"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G486" sqref="G486"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A456" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O499" sqref="O499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5134,10 +5117,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>23</v>
@@ -5160,10 +5143,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -5186,10 +5169,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>27</v>
@@ -5212,10 +5195,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>27</v>
@@ -5238,10 +5221,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>29</v>
@@ -5264,10 +5247,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>29</v>
@@ -5284,16 +5267,16 @@
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -5310,16 +5293,16 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -5342,10 +5325,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>31</v>
@@ -5368,10 +5351,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>31</v>
@@ -5394,10 +5377,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>31</v>
@@ -5420,10 +5403,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>31</v>
@@ -5446,10 +5429,10 @@
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>31</v>
@@ -5472,10 +5455,10 @@
         <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>31</v>
@@ -5498,10 +5481,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>31</v>
@@ -5524,10 +5507,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>31</v>
@@ -5550,10 +5533,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>31</v>
@@ -5576,10 +5559,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>31</v>
@@ -5602,10 +5585,10 @@
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>31</v>
@@ -5628,10 +5611,10 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>31</v>
@@ -5654,10 +5637,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>31</v>
@@ -5680,10 +5663,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>31</v>
@@ -5706,10 +5689,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>31</v>
@@ -11195,7 +11178,7 @@
     </row>
     <row r="238" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>203</v>
@@ -11222,7 +11205,7 @@
     </row>
     <row r="239" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>203</v>
@@ -18053,37 +18036,37 @@
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A492" s="6" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C492" s="6" t="str">
         <f t="shared" si="12"/>
         <v>LRCCW</v>
       </c>
       <c r="D492" s="11" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E492" s="6" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F492" s="6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G492" s="6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C493" s="1" t="str">
         <f t="shared" si="12"/>
@@ -18093,43 +18076,43 @@
         <v>902</v>
       </c>
       <c r="E493" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C494" s="1" t="str">
         <f t="shared" si="12"/>
         <v>LRTWCC</v>
       </c>
       <c r="D494" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E494" s="1" t="s">
         <v>1067</v>
       </c>
-      <c r="E494" s="1" t="s">
-        <v>1068</v>
-      </c>
       <c r="F494" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.2">
@@ -18144,19 +18127,19 @@
         <v>EBART</v>
       </c>
       <c r="D495" s="9" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="E495" s="1" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="F495" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G495" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="H495" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="496" spans="1:8" x14ac:dyDescent="0.2">
@@ -18215,28 +18198,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -18267,7 +18250,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B3" s="1">
         <v>1120</v>
@@ -18276,7 +18259,7 @@
         <v>952</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -18293,7 +18276,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B4" s="1">
         <v>555</v>
@@ -18302,7 +18285,7 @@
         <v>471.75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -18319,7 +18302,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B5" s="1">
         <v>560</v>
@@ -18328,7 +18311,7 @@
         <v>476</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -18371,7 +18354,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B7" s="1">
         <v>784</v>
@@ -18380,7 +18363,7 @@
         <v>666</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -18423,7 +18406,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B9" s="1">
         <v>900</v>
@@ -18432,7 +18415,7 @@
         <v>770</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -18449,7 +18432,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B10" s="1">
         <v>943</v>
@@ -18458,7 +18441,7 @@
         <v>802</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -18475,7 +18458,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B11" s="1">
         <v>952</v>
@@ -18484,7 +18467,7 @@
         <v>809</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -18527,7 +18510,7 @@
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B13" s="20">
         <v>1008</v>
@@ -18536,7 +18519,7 @@
         <v>857</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -18579,7 +18562,7 @@
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B15" s="20">
         <v>70</v>
@@ -18588,7 +18571,7 @@
         <v>59.5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -18657,7 +18640,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B18" s="1">
         <v>1444</v>
@@ -18666,7 +18649,7 @@
         <v>1228</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -18683,7 +18666,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B19" s="1">
         <v>1502</v>
@@ -18692,7 +18675,7 @@
         <v>1276.7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -18709,7 +18692,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="B20" s="1">
         <v>1841</v>
@@ -18718,7 +18701,7 @@
         <v>1564.85</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -18735,7 +18718,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B21" s="1">
         <v>400</v>
@@ -18744,7 +18727,7 @@
         <v>340</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -18761,7 +18744,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B22" s="17">
         <v>450</v>
@@ -18770,7 +18753,7 @@
         <v>382.5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -18787,7 +18770,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B23" s="1">
         <v>250</v>
@@ -18796,7 +18779,7 @@
         <v>212.5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -18813,7 +18796,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B24" s="1">
         <v>275</v>
@@ -18822,7 +18805,7 @@
         <v>233.75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -18891,7 +18874,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B27" s="1">
         <v>298</v>
@@ -18900,7 +18883,7 @@
         <v>253</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18917,7 +18900,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B28" s="1">
         <v>357</v>
@@ -18926,7 +18909,7 @@
         <v>303</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -18943,7 +18926,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B29" s="1">
         <v>476</v>
@@ -18952,7 +18935,7 @@
         <v>404</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -19021,7 +19004,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B32" s="1">
         <v>94</v>
@@ -19030,7 +19013,7 @@
         <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -19073,7 +19056,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B34" s="1">
         <v>80</v>
@@ -19082,7 +19065,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -19099,7 +19082,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B35" s="1">
         <v>80</v>
@@ -19108,7 +19091,7 @@
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -19177,7 +19160,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B38" s="1">
         <v>45</v>
@@ -19186,7 +19169,7 @@
         <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -19255,7 +19238,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B41" s="1">
         <v>63</v>
@@ -19264,7 +19247,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -19411,7 +19394,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B47" s="1">
         <v>94</v>
@@ -19420,7 +19403,7 @@
         <v>79</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -19489,7 +19472,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B50" s="1">
         <v>63</v>
@@ -19498,7 +19481,7 @@
         <v>53</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -19567,7 +19550,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B53" s="1">
         <v>28</v>
@@ -19576,7 +19559,7 @@
         <v>23</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -19593,7 +19576,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B54" s="1">
         <v>200</v>
@@ -19619,7 +19602,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B55" s="1">
         <v>400</v>
@@ -19645,7 +19628,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B56" s="1">
         <v>450</v>
@@ -19654,7 +19637,7 @@
         <v>382.5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -19671,7 +19654,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B57" s="1">
         <v>171</v>
@@ -19681,7 +19664,7 @@
         <v>145.35</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -19698,7 +19681,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B58" s="1">
         <v>342</v>
@@ -19708,7 +19691,7 @@
         <v>290.7</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -19725,7 +19708,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B59" s="1">
         <v>513</v>
@@ -19735,7 +19718,7 @@
         <v>436.05</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -19752,7 +19735,7 @@
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B60" s="18">
         <v>89</v>
@@ -19761,7 +19744,7 @@
         <v>75.649999999999991</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -19778,7 +19761,7 @@
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B61" s="20">
         <v>318</v>
@@ -19787,7 +19770,7 @@
         <v>270.3</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E61" s="20">
         <v>0</v>

</xml_diff>

<commit_message>
Update to Dumbarton Rail vehicle type and capacity
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3682" uniqueCount="1118">
   <si>
     <t>Name</t>
   </si>
@@ -3369,6 +3369,12 @@
   </si>
   <si>
     <t>120_YELLOWE</t>
+  </si>
+  <si>
+    <t>DBRail 4 car</t>
+  </si>
+  <si>
+    <t>134_DBRail</t>
   </si>
 </sst>
 </file>
@@ -4281,8 +4287,8 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4499,7 +4505,7 @@
         <v>912</v>
       </c>
       <c r="C19" t="s">
-        <v>912</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -5016,11 +5022,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H498"/>
+  <dimension ref="A1:H499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A498" sqref="A498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17615,7 +17621,7 @@
         <v>203</v>
       </c>
       <c r="C476" s="4" t="str">
-        <f t="shared" ref="C476:C497" si="12">RIGHT($A476,LEN($A476)-FIND("_",$A476))</f>
+        <f t="shared" ref="C476:C498" si="12">RIGHT($A476,LEN($A476)-FIND("_",$A476))</f>
         <v>L</v>
       </c>
       <c r="D476" s="12" t="s">
@@ -18203,27 +18209,53 @@
     </row>
     <row r="498" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A498" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B498" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="C498" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="D498" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="E498" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="F498" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G498" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H498" s="1" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A499" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B498" s="1" t="s">
+      <c r="B499" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C498" s="1" t="s">
+      <c r="C499" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D498" s="9" t="s">
+      <c r="D499" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E498" s="1" t="s">
+      <c r="E499" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F498" s="1" t="s">
+      <c r="F499" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G498" s="1" t="s">
+      <c r="G499" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H498" s="1" t="s">
+      <c r="H499" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -18235,11 +18267,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18775,41 +18807,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="B21" s="1">
-        <v>400</v>
-      </c>
-      <c r="C21" s="17">
-        <v>340</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="E21" s="1">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B21" s="20">
+        <v>523</v>
+      </c>
+      <c r="C21" s="20">
+        <v>444</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E21" s="20">
         <v>0</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="20">
         <v>0</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="20">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1068</v>
-      </c>
-      <c r="B22" s="17">
-        <v>450</v>
+        <v>929</v>
+      </c>
+      <c r="B22" s="1">
+        <v>400</v>
       </c>
       <c r="C22" s="17">
-        <v>382.5</v>
+        <v>340</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>929</v>
@@ -18829,13 +18861,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B23" s="1">
-        <v>250</v>
+        <v>1068</v>
+      </c>
+      <c r="B23" s="17">
+        <v>450</v>
       </c>
       <c r="C23" s="17">
-        <v>212.5</v>
+        <v>382.5</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>929</v>
@@ -18855,13 +18887,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>1069</v>
+        <v>1098</v>
       </c>
       <c r="B24" s="1">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="C24" s="17">
-        <v>233.75</v>
+        <v>212.5</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>929</v>
@@ -18881,16 +18913,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>328</v>
+        <v>1069</v>
       </c>
       <c r="B25" s="1">
-        <v>119</v>
-      </c>
-      <c r="C25" s="1">
-        <v>101</v>
+        <v>275</v>
+      </c>
+      <c r="C25" s="17">
+        <v>233.75</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>328</v>
+        <v>929</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18899,24 +18931,24 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B26" s="1">
-        <v>238</v>
+        <v>119</v>
       </c>
       <c r="C26" s="1">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -18925,24 +18957,24 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H26" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>1042</v>
+        <v>333</v>
       </c>
       <c r="B27" s="1">
-        <v>298</v>
+        <v>238</v>
       </c>
       <c r="C27" s="1">
-        <v>253</v>
+        <v>202</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1042</v>
+        <v>333</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18951,24 +18983,24 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H27" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B28" s="1">
-        <v>357</v>
+        <v>298</v>
       </c>
       <c r="C28" s="1">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -18977,24 +19009,24 @@
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H28" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B29" s="1">
-        <v>476</v>
+        <v>357</v>
       </c>
       <c r="C29" s="1">
-        <v>404</v>
+        <v>303</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -19003,41 +19035,41 @@
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H29" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>265</v>
+        <v>1040</v>
       </c>
       <c r="B30" s="1">
-        <v>94</v>
+        <v>476</v>
       </c>
       <c r="C30" s="1">
-        <v>79</v>
+        <v>404</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>265</v>
+        <v>1040</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1">
-        <v>0.05</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H30" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
       <c r="B31" s="1">
         <v>94</v>
@@ -19046,7 +19078,7 @@
         <v>79</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -19055,15 +19087,15 @@
         <v>0.122</v>
       </c>
       <c r="G31" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H31" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>1039</v>
+        <v>217</v>
       </c>
       <c r="B32" s="1">
         <v>94</v>
@@ -19072,7 +19104,7 @@
         <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1039</v>
+        <v>217</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -19081,41 +19113,41 @@
         <v>0.122</v>
       </c>
       <c r="G32" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H32" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>224</v>
+        <v>1039</v>
       </c>
       <c r="B33" s="1">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>224</v>
+        <v>1039</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="G33" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H33" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>1038</v>
+        <v>224</v>
       </c>
       <c r="B34" s="1">
         <v>80</v>
@@ -19124,7 +19156,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1038</v>
+        <v>224</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -19133,15 +19165,15 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B35" s="1">
         <v>80</v>
@@ -19150,7 +19182,7 @@
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -19159,41 +19191,41 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G35" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H35" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>261</v>
+        <v>1037</v>
       </c>
       <c r="B36" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>261</v>
+        <v>1037</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G36" s="1">
-        <v>6.2E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="B37" s="1">
         <v>45</v>
@@ -19202,7 +19234,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -19211,15 +19243,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>1036</v>
+        <v>230</v>
       </c>
       <c r="B38" s="1">
         <v>45</v>
@@ -19228,7 +19260,7 @@
         <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1036</v>
+        <v>230</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -19237,24 +19269,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H38" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>205</v>
+        <v>1036</v>
       </c>
       <c r="B39" s="1">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C39" s="1">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>205</v>
+        <v>1036</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -19263,15 +19295,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>6.2E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H39" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B40" s="1">
         <v>63</v>
@@ -19280,7 +19312,7 @@
         <v>53</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -19289,15 +19321,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G40" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H40" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>1035</v>
+        <v>207</v>
       </c>
       <c r="B41" s="1">
         <v>63</v>
@@ -19306,7 +19338,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1035</v>
+        <v>207</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -19315,82 +19347,82 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H41" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>36</v>
+        <v>1035</v>
       </c>
       <c r="B42" s="1">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C42" s="1">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>36</v>
+        <v>1035</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G42" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H42" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B43" s="1">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C43" s="1">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G43" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H43" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>325</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>325</v>
+        <v>53</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G44" s="1">
         <v>6.2E-2</v>
@@ -19401,33 +19433,33 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="B45" s="1">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>0.122</v>
+        <v>0</v>
       </c>
       <c r="G45" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H45" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="B46" s="1">
         <v>94</v>
@@ -19436,7 +19468,7 @@
         <v>79</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -19445,15 +19477,15 @@
         <v>0.122</v>
       </c>
       <c r="G46" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H46" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>1034</v>
+        <v>215</v>
       </c>
       <c r="B47" s="1">
         <v>94</v>
@@ -19462,7 +19494,7 @@
         <v>79</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1034</v>
+        <v>215</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -19471,41 +19503,41 @@
         <v>0.122</v>
       </c>
       <c r="G47" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H47" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>234</v>
+        <v>1034</v>
       </c>
       <c r="B48" s="1">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="C48" s="1">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>234</v>
+        <v>1034</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G48" s="1">
-        <v>6.2E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H48" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B49" s="1">
         <v>63</v>
@@ -19514,7 +19546,7 @@
         <v>53</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -19523,15 +19555,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G49" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H49" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>1033</v>
+        <v>235</v>
       </c>
       <c r="B50" s="1">
         <v>63</v>
@@ -19540,7 +19572,7 @@
         <v>53</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1033</v>
+        <v>235</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -19549,50 +19581,50 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G50" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H50" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>906</v>
+        <v>1033</v>
       </c>
       <c r="B51" s="1">
-        <v>800</v>
+        <v>63</v>
       </c>
       <c r="C51" s="1">
-        <v>680</v>
+        <v>53</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>906</v>
+        <v>1033</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H51" s="1">
-        <v>0</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>259</v>
+        <v>906</v>
       </c>
       <c r="B52" s="1">
-        <v>25</v>
+        <v>800</v>
       </c>
       <c r="C52" s="1">
-        <v>21</v>
+        <v>680</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>259</v>
+        <v>906</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -19601,24 +19633,24 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>1032</v>
+        <v>259</v>
       </c>
       <c r="B53" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1032</v>
+        <v>259</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -19635,16 +19667,16 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1099</v>
+        <v>1032</v>
       </c>
       <c r="B54" s="1">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="C54" s="1">
-        <v>170</v>
+        <v>23</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>909</v>
+        <v>1032</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -19653,21 +19685,21 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H54" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1073</v>
+        <v>1099</v>
       </c>
       <c r="B55" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C55" s="1">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>909</v>
@@ -19687,16 +19719,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1059</v>
+        <v>1073</v>
       </c>
       <c r="B56" s="1">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C56" s="1">
-        <v>382.5</v>
+        <v>340</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1097</v>
+        <v>909</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -19713,17 +19745,16 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>1102</v>
+        <v>1059</v>
       </c>
       <c r="B57" s="1">
-        <v>171</v>
-      </c>
-      <c r="C57" s="17">
-        <f t="shared" ref="C57:C59" si="0">B57*0.85</f>
-        <v>145.35</v>
+        <v>450</v>
+      </c>
+      <c r="C57" s="1">
+        <v>382.5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1104</v>
+        <v>1097</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -19732,78 +19763,79 @@
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H57" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B58" s="1">
+        <v>171</v>
+      </c>
+      <c r="C58" s="17">
+        <f t="shared" ref="C58:C60" si="0">B58*0.85</f>
+        <v>145.35</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B59" s="1">
         <v>342</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C59" s="17">
         <f t="shared" si="0"/>
         <v>290.7</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>1105</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="1">
         <v>0</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F59" s="1">
         <v>0</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G59" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H59" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>1103</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B60" s="1">
         <v>513</v>
       </c>
-      <c r="C59" s="17">
+      <c r="C60" s="17">
         <f t="shared" si="0"/>
         <v>436.05</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>1106</v>
-      </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="1">
-        <v>0</v>
-      </c>
-      <c r="G59" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H59" s="1">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B60" s="18">
-        <v>89</v>
-      </c>
-      <c r="C60" s="19">
-        <v>75.649999999999991</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>1107</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -19812,35 +19844,61 @@
         <v>0</v>
       </c>
       <c r="G60" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H60" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B61" s="18">
+        <v>89</v>
+      </c>
+      <c r="C61" s="19">
+        <v>75.649999999999991</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E61" s="1">
         <v>0</v>
       </c>
-      <c r="H60" s="1">
+      <c r="F61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B62" s="20">
         <v>318</v>
       </c>
-      <c r="C61" s="21">
+      <c r="C62" s="21">
         <v>270.3</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D62" s="20" t="s">
         <v>1108</v>
       </c>
-      <c r="E61" s="20">
+      <c r="E62" s="20">
         <v>0</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F62" s="20">
         <v>0</v>
       </c>
-      <c r="G61" s="20">
+      <c r="G62" s="20">
         <v>0</v>
       </c>
-      <c r="H61" s="20">
+      <c r="H62" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Update to Dumbarton Rail vehicle type and capacity"
This reverts commit d0709a6bb53d396757b3edb75835a0091e5fff33.
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\TM1_2015_Base_Network\trn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\trn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3682" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="1116">
   <si>
     <t>Name</t>
   </si>
@@ -3369,12 +3369,6 @@
   </si>
   <si>
     <t>120_YELLOWE</t>
-  </si>
-  <si>
-    <t>DBRail 4 car</t>
-  </si>
-  <si>
-    <t>134_DBRail</t>
   </si>
 </sst>
 </file>
@@ -4287,8 +4281,8 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4505,7 +4499,7 @@
         <v>912</v>
       </c>
       <c r="C19" t="s">
-        <v>1116</v>
+        <v>912</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -5022,11 +5016,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H499"/>
+  <dimension ref="A1:H498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A498" sqref="A498"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17621,7 +17615,7 @@
         <v>203</v>
       </c>
       <c r="C476" s="4" t="str">
-        <f t="shared" ref="C476:C498" si="12">RIGHT($A476,LEN($A476)-FIND("_",$A476))</f>
+        <f t="shared" ref="C476:C497" si="12">RIGHT($A476,LEN($A476)-FIND("_",$A476))</f>
         <v>L</v>
       </c>
       <c r="D476" s="12" t="s">
@@ -18209,53 +18203,27 @@
     </row>
     <row r="498" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A498" s="1" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B498" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="C498" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="D498" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="E498" s="4" t="s">
-        <v>912</v>
+        <v>0</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D498" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="F498" s="1" t="s">
-        <v>1116</v>
+        <v>5</v>
       </c>
       <c r="G498" s="1" t="s">
-        <v>1116</v>
+        <v>6</v>
       </c>
       <c r="H498" s="1" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A499" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B499" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C499" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D499" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E499" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F499" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G499" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H499" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -18267,11 +18235,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:H21"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18807,41 +18775,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B21" s="20">
-        <v>523</v>
-      </c>
-      <c r="C21" s="20">
-        <v>444</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>1116</v>
-      </c>
-      <c r="E21" s="20">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B21" s="1">
+        <v>400</v>
+      </c>
+      <c r="C21" s="17">
+        <v>340</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="1">
         <v>0</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="B22" s="1">
-        <v>400</v>
+        <v>1068</v>
+      </c>
+      <c r="B22" s="17">
+        <v>450</v>
       </c>
       <c r="C22" s="17">
-        <v>340</v>
+        <v>382.5</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>929</v>
@@ -18861,13 +18829,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>1068</v>
-      </c>
-      <c r="B23" s="17">
-        <v>450</v>
+        <v>1098</v>
+      </c>
+      <c r="B23" s="1">
+        <v>250</v>
       </c>
       <c r="C23" s="17">
-        <v>382.5</v>
+        <v>212.5</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>929</v>
@@ -18887,13 +18855,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>1098</v>
+        <v>1069</v>
       </c>
       <c r="B24" s="1">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="C24" s="17">
-        <v>212.5</v>
+        <v>233.75</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>929</v>
@@ -18913,16 +18881,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1069</v>
+        <v>328</v>
       </c>
       <c r="B25" s="1">
-        <v>275</v>
-      </c>
-      <c r="C25" s="17">
-        <v>233.75</v>
+        <v>119</v>
+      </c>
+      <c r="C25" s="1">
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>929</v>
+        <v>328</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -18931,24 +18899,24 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="B26" s="1">
-        <v>119</v>
+        <v>238</v>
       </c>
       <c r="C26" s="1">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -18957,24 +18925,24 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H26" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>333</v>
+        <v>1042</v>
       </c>
       <c r="B27" s="1">
-        <v>238</v>
+        <v>298</v>
       </c>
       <c r="C27" s="1">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>333</v>
+        <v>1042</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -18983,24 +18951,24 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H27" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B28" s="1">
-        <v>298</v>
+        <v>357</v>
       </c>
       <c r="C28" s="1">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -19009,24 +18977,24 @@
         <v>0</v>
       </c>
       <c r="G28" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H28" s="1">
         <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="H28" s="1">
-        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B29" s="1">
-        <v>357</v>
+        <v>476</v>
       </c>
       <c r="C29" s="1">
-        <v>303</v>
+        <v>404</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -19035,41 +19003,41 @@
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H29" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>1040</v>
+        <v>265</v>
       </c>
       <c r="B30" s="1">
-        <v>476</v>
+        <v>94</v>
       </c>
       <c r="C30" s="1">
-        <v>404</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1040</v>
+        <v>265</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="G30" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="H30" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1">
         <v>94</v>
@@ -19078,7 +19046,7 @@
         <v>79</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -19087,15 +19055,15 @@
         <v>0.122</v>
       </c>
       <c r="G31" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H31" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>217</v>
+        <v>1039</v>
       </c>
       <c r="B32" s="1">
         <v>94</v>
@@ -19104,7 +19072,7 @@
         <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>217</v>
+        <v>1039</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -19113,41 +19081,41 @@
         <v>0.122</v>
       </c>
       <c r="G32" s="1">
-        <v>0.04</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H32" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>1039</v>
+        <v>224</v>
       </c>
       <c r="B33" s="1">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C33" s="1">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1039</v>
+        <v>224</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0.122</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G33" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H33" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>224</v>
+        <v>1038</v>
       </c>
       <c r="B34" s="1">
         <v>80</v>
@@ -19156,7 +19124,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>224</v>
+        <v>1038</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -19165,15 +19133,15 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H34" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B35" s="1">
         <v>80</v>
@@ -19182,7 +19150,7 @@
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -19191,41 +19159,41 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="G35" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H35" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>1037</v>
+        <v>261</v>
       </c>
       <c r="B36" s="1">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1037</v>
+        <v>261</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>0.10199999999999999</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="B37" s="1">
         <v>45</v>
@@ -19234,7 +19202,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -19243,15 +19211,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H37" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>230</v>
+        <v>1036</v>
       </c>
       <c r="B38" s="1">
         <v>45</v>
@@ -19260,7 +19228,7 @@
         <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>230</v>
+        <v>1036</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -19269,24 +19237,24 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H38" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>1036</v>
+        <v>205</v>
       </c>
       <c r="B39" s="1">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1036</v>
+        <v>205</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -19295,15 +19263,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>0.04</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B40" s="1">
         <v>63</v>
@@ -19312,7 +19280,7 @@
         <v>53</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -19321,15 +19289,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G40" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H40" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>207</v>
+        <v>1035</v>
       </c>
       <c r="B41" s="1">
         <v>63</v>
@@ -19338,7 +19306,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>207</v>
+        <v>1035</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -19347,82 +19315,82 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H41" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>1035</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1">
+        <v>75</v>
+      </c>
+      <c r="C42" s="1">
         <v>63</v>
       </c>
-      <c r="C42" s="1">
-        <v>53</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>1035</v>
+        <v>36</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="G42" s="1">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="H42" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B43" s="1">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H43" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>325</v>
       </c>
       <c r="B44" s="1">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C44" s="1">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>53</v>
+        <v>325</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
         <v>6.2E-2</v>
@@ -19433,33 +19401,33 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>325</v>
+        <v>245</v>
       </c>
       <c r="B45" s="1">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>325</v>
+        <v>245</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
       </c>
       <c r="F45" s="1">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="G45" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H45" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="B46" s="1">
         <v>94</v>
@@ -19468,7 +19436,7 @@
         <v>79</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -19477,15 +19445,15 @@
         <v>0.122</v>
       </c>
       <c r="G46" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H46" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>215</v>
+        <v>1034</v>
       </c>
       <c r="B47" s="1">
         <v>94</v>
@@ -19494,7 +19462,7 @@
         <v>79</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>215</v>
+        <v>1034</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -19503,41 +19471,41 @@
         <v>0.122</v>
       </c>
       <c r="G47" s="1">
-        <v>0.04</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H47" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>1034</v>
+        <v>234</v>
       </c>
       <c r="B48" s="1">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C48" s="1">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1034</v>
+        <v>234</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>0.122</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G48" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H48" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B49" s="1">
         <v>63</v>
@@ -19546,7 +19514,7 @@
         <v>53</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -19555,15 +19523,15 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G49" s="1">
-        <v>6.2E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H49" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>235</v>
+        <v>1033</v>
       </c>
       <c r="B50" s="1">
         <v>63</v>
@@ -19572,7 +19540,7 @@
         <v>53</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>235</v>
+        <v>1033</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -19581,50 +19549,50 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G50" s="1">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="H50" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>1033</v>
+        <v>906</v>
       </c>
       <c r="B51" s="1">
-        <v>63</v>
+        <v>800</v>
       </c>
       <c r="C51" s="1">
-        <v>53</v>
+        <v>680</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1033</v>
+        <v>906</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>906</v>
+        <v>259</v>
       </c>
       <c r="B52" s="1">
-        <v>800</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1">
-        <v>680</v>
+        <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>906</v>
+        <v>259</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -19633,24 +19601,24 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>0</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>259</v>
+        <v>1032</v>
       </c>
       <c r="B53" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C53" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>259</v>
+        <v>1032</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -19667,16 +19635,16 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>1032</v>
+        <v>1099</v>
       </c>
       <c r="B54" s="1">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1">
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1032</v>
+        <v>909</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -19685,21 +19653,21 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H54" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>1099</v>
+        <v>1073</v>
       </c>
       <c r="B55" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C55" s="1">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>909</v>
@@ -19719,16 +19687,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1073</v>
+        <v>1059</v>
       </c>
       <c r="B56" s="1">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="C56" s="1">
-        <v>340</v>
+        <v>382.5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>909</v>
+        <v>1097</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -19745,16 +19713,17 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>1059</v>
+        <v>1102</v>
       </c>
       <c r="B57" s="1">
-        <v>450</v>
-      </c>
-      <c r="C57" s="1">
-        <v>382.5</v>
+        <v>171</v>
+      </c>
+      <c r="C57" s="17">
+        <f t="shared" ref="C57:C59" si="0">B57*0.85</f>
+        <v>145.35</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1097</v>
+        <v>1104</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -19763,25 +19732,25 @@
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>0</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H57" s="1">
-        <v>0</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>1102</v>
+        <v>1070</v>
       </c>
       <c r="B58" s="1">
-        <v>171</v>
+        <v>342</v>
       </c>
       <c r="C58" s="17">
-        <f t="shared" ref="C58:C60" si="0">B58*0.85</f>
-        <v>145.35</v>
+        <f t="shared" si="0"/>
+        <v>290.7</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -19790,25 +19759,25 @@
         <v>0</v>
       </c>
       <c r="G58" s="1">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H58" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>1070</v>
+        <v>1103</v>
       </c>
       <c r="B59" s="1">
-        <v>342</v>
+        <v>513</v>
       </c>
       <c r="C59" s="17">
         <f t="shared" si="0"/>
-        <v>290.7</v>
+        <v>436.05</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -19817,25 +19786,24 @@
         <v>0</v>
       </c>
       <c r="G59" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H59" s="1">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B60" s="1">
-        <v>513</v>
-      </c>
-      <c r="C60" s="17">
-        <f t="shared" si="0"/>
-        <v>436.05</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>1106</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B60" s="18">
+        <v>89</v>
+      </c>
+      <c r="C60" s="19">
+        <v>75.649999999999991</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>1107</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -19844,61 +19812,35 @@
         <v>0</v>
       </c>
       <c r="G60" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="H60" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B61" s="18">
-        <v>89</v>
-      </c>
-      <c r="C61" s="19">
-        <v>75.649999999999991</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>1107</v>
-      </c>
-      <c r="E61" s="1">
+      <c r="A61" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B61" s="20">
+        <v>318</v>
+      </c>
+      <c r="C61" s="21">
+        <v>270.3</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E61" s="20">
         <v>0</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="20">
         <v>0</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="20">
         <v>0</v>
       </c>
-      <c r="H61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B62" s="20">
-        <v>318</v>
-      </c>
-      <c r="C62" s="21">
-        <v>270.3</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E62" s="20">
-        <v>0</v>
-      </c>
-      <c r="F62" s="20">
-        <v>0</v>
-      </c>
-      <c r="G62" s="20">
-        <v>0</v>
-      </c>
-      <c r="H62" s="20">
+      <c r="H61" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add transformative project SR85's capacity info
Anup wanted delay-per-stop time reflected, and the method for adding capacity via project doe not allow for changing that attribute. So I have added it to the base files
</commit_message>
<xml_diff>
--- a/trn/TransitCapacity.xlsx
+++ b/trn/TransitCapacity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19755" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="transitPrefixToVehicle" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="1120">
   <si>
     <t>Name</t>
   </si>
@@ -3369,6 +3369,18 @@
   </si>
   <si>
     <t>120_YELLOWE</t>
+  </si>
+  <si>
+    <t>SR85 LRV</t>
+  </si>
+  <si>
+    <t>SR85 Light Rail Vehicle</t>
+  </si>
+  <si>
+    <t>115_</t>
+  </si>
+  <si>
+    <t>SR85 Rail</t>
   </si>
 </sst>
 </file>
@@ -4278,11 +4290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4404,77 +4416,77 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C11" t="s">
-        <v>261</v>
+      <c r="A11" s="20" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>924</v>
+        <v>1027</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>1026</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B13" t="s">
-        <v>922</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>1071</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1025</v>
+        <v>923</v>
       </c>
       <c r="B14" t="s">
-        <v>1024</v>
+        <v>922</v>
       </c>
       <c r="C14" t="s">
-        <v>261</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>921</v>
+        <v>1025</v>
       </c>
       <c r="B15" t="s">
-        <v>920</v>
+        <v>1024</v>
       </c>
       <c r="C15" t="s">
-        <v>920</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B16" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C16" t="s">
-        <v>906</v>
+        <v>920</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="B17" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C17" t="s">
         <v>906</v>
@@ -4482,10 +4494,10 @@
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B18" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C18" t="s">
         <v>906</v>
@@ -4493,54 +4505,54 @@
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B19" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C19" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B20" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C20" t="s">
-        <v>1072</v>
+        <v>912</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B21" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="C21" t="s">
-        <v>1059</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1023</v>
+        <v>908</v>
       </c>
       <c r="B22" t="s">
-        <v>1022</v>
+        <v>907</v>
       </c>
       <c r="C22" t="s">
-        <v>261</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B23" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C23" t="s">
         <v>261</v>
@@ -4548,10 +4560,10 @@
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B24" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C24" t="s">
         <v>261</v>
@@ -4559,10 +4571,10 @@
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B25" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C25" t="s">
         <v>261</v>
@@ -4570,10 +4582,10 @@
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B26" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C26" t="s">
         <v>261</v>
@@ -4581,10 +4593,10 @@
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B27" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="C27" t="s">
         <v>261</v>
@@ -4592,10 +4604,10 @@
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B28" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C28" t="s">
         <v>261</v>
@@ -4603,32 +4615,32 @@
     </row>
     <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B29" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="C29" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B30" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C30" t="s">
-        <v>205</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B31" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="C31" t="s">
         <v>205</v>
@@ -4636,10 +4648,10 @@
     </row>
     <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B32" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C32" t="s">
         <v>205</v>
@@ -4647,10 +4659,10 @@
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B33" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C33" t="s">
         <v>205</v>
@@ -4658,10 +4670,10 @@
     </row>
     <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B34" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C34" t="s">
         <v>205</v>
@@ -4669,10 +4681,10 @@
     </row>
     <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B35" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C35" t="s">
         <v>205</v>
@@ -4680,10 +4692,10 @@
     </row>
     <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B36" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="C36" t="s">
         <v>205</v>
@@ -4691,10 +4703,10 @@
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B37" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="C37" t="s">
         <v>205</v>
@@ -4702,10 +4714,10 @@
     </row>
     <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B38" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C38" t="s">
         <v>205</v>
@@ -4713,10 +4725,10 @@
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B39" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C39" t="s">
         <v>205</v>
@@ -4724,10 +4736,10 @@
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B40" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C40" t="s">
         <v>205</v>
@@ -4735,10 +4747,10 @@
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B41" t="s">
-        <v>979</v>
+        <v>986</v>
       </c>
       <c r="C41" t="s">
         <v>205</v>
@@ -4746,10 +4758,10 @@
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B42" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="C42" t="s">
         <v>205</v>
@@ -4757,10 +4769,10 @@
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="B43" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C43" t="s">
         <v>205</v>
@@ -4768,10 +4780,10 @@
     </row>
     <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B44" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C44" t="s">
         <v>205</v>
@@ -4779,10 +4791,10 @@
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B45" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="C45" t="s">
         <v>205</v>
@@ -4790,10 +4802,10 @@
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B46" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C46" t="s">
         <v>205</v>
@@ -4801,10 +4813,10 @@
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B47" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C47" t="s">
         <v>205</v>
@@ -4812,10 +4824,10 @@
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="B48" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C48" t="s">
         <v>205</v>
@@ -4823,10 +4835,10 @@
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="B49" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C49" t="s">
         <v>205</v>
@@ -4834,10 +4846,10 @@
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B50" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C50" t="s">
         <v>205</v>
@@ -4845,10 +4857,10 @@
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B51" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C51" t="s">
         <v>205</v>
@@ -4856,10 +4868,10 @@
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B52" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="C52" t="s">
         <v>205</v>
@@ -4867,10 +4879,10 @@
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B53" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C53" t="s">
         <v>205</v>
@@ -4878,10 +4890,10 @@
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B54" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="C54" t="s">
         <v>205</v>
@@ -4889,7 +4901,7 @@
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B55" t="s">
         <v>958</v>
@@ -4900,10 +4912,10 @@
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B56" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C56" t="s">
         <v>205</v>
@@ -4911,10 +4923,10 @@
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B57" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="C57" t="s">
         <v>205</v>
@@ -4922,7 +4934,7 @@
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B58" t="s">
         <v>953</v>
@@ -4933,10 +4945,10 @@
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="B59" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C59" t="s">
         <v>205</v>
@@ -4944,10 +4956,10 @@
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B60" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C60" t="s">
         <v>205</v>
@@ -4955,10 +4967,10 @@
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="B61" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C61" t="s">
         <v>205</v>
@@ -4966,10 +4978,10 @@
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="B62" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
       <c r="C62" t="s">
         <v>205</v>
@@ -4977,10 +4989,10 @@
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B63" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C63" t="s">
         <v>205</v>
@@ -4988,10 +5000,10 @@
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B64" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="C64" t="s">
         <v>205</v>
@@ -4999,12 +5011,23 @@
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>943</v>
+      </c>
+      <c r="B65" t="s">
+        <v>942</v>
+      </c>
+      <c r="C65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>1031</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>1</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>1030</v>
       </c>
     </row>
@@ -5018,9 +5041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H498"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18235,11 +18258,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19792,18 +19815,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B60" s="18">
-        <v>89</v>
-      </c>
-      <c r="C60" s="19">
-        <v>75.649999999999991</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>1107</v>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B60" s="1">
+        <v>90</v>
+      </c>
+      <c r="C60" s="17">
+        <v>77</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1117</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -19812,35 +19835,61 @@
         <v>0</v>
       </c>
       <c r="G60" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B61" s="18">
+        <v>89</v>
+      </c>
+      <c r="C61" s="19">
+        <v>75.649999999999991</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E61" s="1">
         <v>0</v>
       </c>
-      <c r="H60" s="1">
+      <c r="F61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B62" s="20">
         <v>318</v>
       </c>
-      <c r="C61" s="21">
+      <c r="C62" s="21">
         <v>270.3</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D62" s="20" t="s">
         <v>1108</v>
       </c>
-      <c r="E61" s="20">
+      <c r="E62" s="20">
         <v>0</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F62" s="20">
         <v>0</v>
       </c>
-      <c r="G61" s="20">
+      <c r="G62" s="20">
         <v>0</v>
       </c>
-      <c r="H61" s="20">
+      <c r="H62" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>